<commit_message>
Commit Auto (Fri May 31 17:58:36     2024)
</commit_message>
<xml_diff>
--- a/SoftIce/ice/Фростор 19.04.24.xlsx
+++ b/SoftIce/ice/Фростор 19.04.24.xlsx
@@ -2740,7 +2740,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2870,6 +2870,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4008,9 +4014,6 @@
     <xf numFmtId="49" fontId="37" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="35" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4135,6 +4138,36 @@
     <xf numFmtId="3" fontId="35" fillId="22" borderId="38" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="35" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="18" borderId="38" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="18" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="18" borderId="45" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="18" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="18" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="67" fillId="16" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4204,35 +4237,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="37" fillId="23" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="18" borderId="38" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="30" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="18" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="18" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="18" borderId="45" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="18" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="30" fillId="18" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="31">
@@ -4373,7 +4379,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AA1ACFBB-3266-4B51-A6C2-4B4B665E041A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA1ACFBB-3266-4B51-A6C2-4B4B665E041A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4423,7 +4429,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1D66AAD1-5BAC-4739-B721-BD89D97D43C4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D66AAD1-5BAC-4739-B721-BD89D97D43C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4473,7 +4479,7 @@
         <xdr:cNvPr id="9" name="Рисунок 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{505DA658-ADC6-4FE4-B792-BB96AD9F6093}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{505DA658-ADC6-4FE4-B792-BB96AD9F6093}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4523,7 +4529,7 @@
         <xdr:cNvPr id="67" name="Рисунок 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E77DE0E3-172F-4595-BE6F-F3CEDB186E65}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E77DE0E3-172F-4595-BE6F-F3CEDB186E65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4573,7 +4579,7 @@
         <xdr:cNvPr id="11" name="Рисунок 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79A97C94-FE7C-45A0-B7B8-B036BAB4F3FC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79A97C94-FE7C-45A0-B7B8-B036BAB4F3FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4623,7 +4629,7 @@
         <xdr:cNvPr id="13" name="Рисунок 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08E9F54E-76F7-46D1-83A5-B4A81EF2460A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08E9F54E-76F7-46D1-83A5-B4A81EF2460A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4673,7 +4679,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{44CA116D-5A8E-41AA-90C2-8CB1A9920212}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44CA116D-5A8E-41AA-90C2-8CB1A9920212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4723,7 +4729,7 @@
         <xdr:cNvPr id="72" name="Рисунок 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{46FBD2BD-0D57-40BD-BFEC-FD7735425613}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46FBD2BD-0D57-40BD-BFEC-FD7735425613}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4773,7 +4779,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B4C9062-0C12-49F7-90BD-5DDE7288926E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B4C9062-0C12-49F7-90BD-5DDE7288926E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4823,7 +4829,7 @@
         <xdr:cNvPr id="29" name="Рисунок 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4ACADB7-E340-44C6-BC60-B79F691D3F05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4ACADB7-E340-44C6-BC60-B79F691D3F05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4873,7 +4879,7 @@
         <xdr:cNvPr id="31" name="Рисунок 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38E193AA-0463-418B-A287-51BDDB233366}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E193AA-0463-418B-A287-51BDDB233366}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4923,7 +4929,7 @@
         <xdr:cNvPr id="73" name="Рисунок 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D6263A97-EA2C-4AFF-8586-A26B64605C34}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6263A97-EA2C-4AFF-8586-A26B64605C34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4973,7 +4979,7 @@
         <xdr:cNvPr id="45" name="Рисунок 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5365ADE7-524E-4E5F-B716-EB3E2E2A778C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5365ADE7-524E-4E5F-B716-EB3E2E2A778C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5023,7 +5029,7 @@
         <xdr:cNvPr id="74" name="Рисунок 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{506B0900-2101-4BE5-B706-D446268DE6AC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{506B0900-2101-4BE5-B706-D446268DE6AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5073,7 +5079,7 @@
         <xdr:cNvPr id="47" name="Рисунок 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{17373A6B-76BB-4D04-AF15-68C877857DD0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17373A6B-76BB-4D04-AF15-68C877857DD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5123,7 +5129,7 @@
         <xdr:cNvPr id="49" name="Рисунок 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CC85C092-C4D8-486A-BB15-FAD874504601}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC85C092-C4D8-486A-BB15-FAD874504601}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5173,7 +5179,7 @@
         <xdr:cNvPr id="76" name="Рисунок 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD4298F1-43FE-40C0-ACEA-7D8E8E9B0F37}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD4298F1-43FE-40C0-ACEA-7D8E8E9B0F37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5223,7 +5229,7 @@
         <xdr:cNvPr id="78" name="Рисунок 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5305F545-6052-4D32-8FDE-597AAA8618DD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5305F545-6052-4D32-8FDE-597AAA8618DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5273,7 +5279,7 @@
         <xdr:cNvPr id="79" name="Рисунок 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{649E095E-F9C8-4240-A2CE-5CB04D065F73}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{649E095E-F9C8-4240-A2CE-5CB04D065F73}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5323,7 +5329,7 @@
         <xdr:cNvPr id="81" name="Рисунок 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84E66361-F1C9-48C5-97C5-7989E7256677}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84E66361-F1C9-48C5-97C5-7989E7256677}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5373,7 +5379,7 @@
         <xdr:cNvPr id="82" name="Рисунок 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F33FED6A-AB08-424E-839A-92BBE28467EF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F33FED6A-AB08-424E-839A-92BBE28467EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5423,7 +5429,7 @@
         <xdr:cNvPr id="83" name="Рисунок 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2793BF4B-E02F-4B54-B25D-3E971201BF8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2793BF4B-E02F-4B54-B25D-3E971201BF8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5473,7 +5479,7 @@
         <xdr:cNvPr id="86" name="Рисунок 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D1F6617C-8859-4576-A17A-8F217C4EF54D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F6617C-8859-4576-A17A-8F217C4EF54D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5523,7 +5529,7 @@
         <xdr:cNvPr id="88" name="Рисунок 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4FC5458D-3083-4153-B36E-BA187DF72AFF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FC5458D-3083-4153-B36E-BA187DF72AFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5573,7 +5579,7 @@
         <xdr:cNvPr id="89" name="Рисунок 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4007AB70-8047-4149-B0FB-4B51136B8E63}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4007AB70-8047-4149-B0FB-4B51136B8E63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5623,7 +5629,7 @@
         <xdr:cNvPr id="91" name="Рисунок 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7EAD394-6B87-49D0-AD64-F146DD8F480E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7EAD394-6B87-49D0-AD64-F146DD8F480E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5673,7 +5679,7 @@
         <xdr:cNvPr id="93" name="Рисунок 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55F031BE-AD15-4B72-983B-E5B8128B6A21}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55F031BE-AD15-4B72-983B-E5B8128B6A21}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5723,7 +5729,7 @@
         <xdr:cNvPr id="95" name="Рисунок 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B85DE6AD-C034-4AAC-A74F-1E36B2375F9C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B85DE6AD-C034-4AAC-A74F-1E36B2375F9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5773,7 +5779,7 @@
         <xdr:cNvPr id="96" name="Рисунок 95">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{46A156F9-264B-4A3A-8FFD-ABC238E91EC8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46A156F9-264B-4A3A-8FFD-ABC238E91EC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5823,7 +5829,7 @@
         <xdr:cNvPr id="98" name="Рисунок 97">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31F77DA2-B3BA-48A6-A56C-E97171595A59}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31F77DA2-B3BA-48A6-A56C-E97171595A59}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5873,7 +5879,7 @@
         <xdr:cNvPr id="100" name="Рисунок 99">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9ACC027-E330-49E4-95F6-97B8ABBD43D5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9ACC027-E330-49E4-95F6-97B8ABBD43D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5923,7 +5929,7 @@
         <xdr:cNvPr id="101" name="Рисунок 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D277B565-53A9-4844-B749-A173258F13A6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D277B565-53A9-4844-B749-A173258F13A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5973,7 +5979,7 @@
         <xdr:cNvPr id="102" name="Рисунок 101">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A043CCF-A8C5-4684-AE89-0C3524E76DB7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A043CCF-A8C5-4684-AE89-0C3524E76DB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6023,7 +6029,7 @@
         <xdr:cNvPr id="104" name="Рисунок 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7D4224A9-2F80-4EB6-B209-C17281907B3E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D4224A9-2F80-4EB6-B209-C17281907B3E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6073,7 +6079,7 @@
         <xdr:cNvPr id="106" name="Рисунок 105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84C01A40-FA55-426C-A175-52B7F6FB6094}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C01A40-FA55-426C-A175-52B7F6FB6094}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6123,7 +6129,7 @@
         <xdr:cNvPr id="107" name="Рисунок 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61D93B6E-243C-4F3B-8C05-EF7F06238827}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D93B6E-243C-4F3B-8C05-EF7F06238827}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6173,7 +6179,7 @@
         <xdr:cNvPr id="109" name="Рисунок 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E609CDBB-8C12-4549-BEE5-0826E8E4B88E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E609CDBB-8C12-4549-BEE5-0826E8E4B88E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6223,7 +6229,7 @@
         <xdr:cNvPr id="110" name="Рисунок 109">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{98CDDAA0-3942-432D-B14E-48EEFF74AE76}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98CDDAA0-3942-432D-B14E-48EEFF74AE76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6273,7 +6279,7 @@
         <xdr:cNvPr id="111" name="Рисунок 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29875149-6284-464F-88D4-9754C07BB095}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29875149-6284-464F-88D4-9754C07BB095}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6323,7 +6329,7 @@
         <xdr:cNvPr id="113" name="Рисунок 112">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2A6C9406-B1DE-4862-B9B3-0B828833B5CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A6C9406-B1DE-4862-B9B3-0B828833B5CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6373,7 +6379,7 @@
         <xdr:cNvPr id="114" name="Рисунок 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A999D5CB-7B5D-43A4-A1A0-CA90C431ABA5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A999D5CB-7B5D-43A4-A1A0-CA90C431ABA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6423,7 +6429,7 @@
         <xdr:cNvPr id="44" name="Picture 1029">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ADBEA432-E081-428F-8714-63084FA11034}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADBEA432-E081-428F-8714-63084FA11034}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6502,7 +6508,7 @@
         <xdr:cNvPr id="2" name="Picture 1029">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6576,7 +6582,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24049225-B489-43B7-BDB7-E9C104CBE58C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24049225-B489-43B7-BDB7-E9C104CBE58C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6626,7 +6632,7 @@
         <xdr:cNvPr id="22" name="Рисунок 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DBD1F57F-2FB2-41EB-9B4B-A6D25C663FA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD1F57F-2FB2-41EB-9B4B-A6D25C663FA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6676,7 +6682,7 @@
         <xdr:cNvPr id="12" name="Рисунок 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9DE3604-5C92-4E44-9D03-6A2370D2D838}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9DE3604-5C92-4E44-9D03-6A2370D2D838}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6726,7 +6732,7 @@
         <xdr:cNvPr id="25" name="Рисунок 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD5A47B7-2A7D-4CF2-A9AD-76B1936DA0EA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5A47B7-2A7D-4CF2-A9AD-76B1936DA0EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6776,7 +6782,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D00256DC-24EA-4A3B-B959-66E63D67A33D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D00256DC-24EA-4A3B-B959-66E63D67A33D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6826,7 +6832,7 @@
         <xdr:cNvPr id="29" name="Рисунок 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04126507-E026-4C44-9DF0-B777B39F24C4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04126507-E026-4C44-9DF0-B777B39F24C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6866,8 +6872,8 @@
       <xdr:rowOff>103908</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>87256</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2338620</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>1257299</xdr:rowOff>
     </xdr:to>
@@ -6876,7 +6882,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07222039-639E-48CE-A508-42EE22195058}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07222039-639E-48CE-A508-42EE22195058}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6916,8 +6922,8 @@
       <xdr:rowOff>207818</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>87256</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2338620</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>1361209</xdr:rowOff>
     </xdr:to>
@@ -6926,7 +6932,7 @@
         <xdr:cNvPr id="32" name="Рисунок 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{03DC5BCE-DF05-4E02-B799-9BFCD9E339F6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03DC5BCE-DF05-4E02-B799-9BFCD9E339F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6976,7 +6982,7 @@
         <xdr:cNvPr id="33" name="Рисунок 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{98E588EC-6BB7-40E9-8A02-BB6D75E25CAF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E588EC-6BB7-40E9-8A02-BB6D75E25CAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7026,7 +7032,7 @@
         <xdr:cNvPr id="34" name="Рисунок 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2AFC1F9C-C6C4-4F43-926C-C35E93E87BCD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AFC1F9C-C6C4-4F43-926C-C35E93E87BCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7066,8 +7072,8 @@
       <xdr:rowOff>346364</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>52619</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2303983</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>1499755</xdr:rowOff>
     </xdr:to>
@@ -7076,7 +7082,7 @@
         <xdr:cNvPr id="35" name="Рисунок 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84D8FA04-08A8-4568-AA26-420F4782336B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84D8FA04-08A8-4568-AA26-420F4782336B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7116,8 +7122,8 @@
       <xdr:rowOff>311727</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>69938</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2321302</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>1465118</xdr:rowOff>
     </xdr:to>
@@ -7126,7 +7132,7 @@
         <xdr:cNvPr id="36" name="Рисунок 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D485DEF-63D2-4A35-8991-9D8BF3E5FA6D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D485DEF-63D2-4A35-8991-9D8BF3E5FA6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7176,7 +7182,7 @@
         <xdr:cNvPr id="21" name="Рисунок 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63FB1715-A81A-49F6-8E5F-0E233DED912D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63FB1715-A81A-49F6-8E5F-0E233DED912D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7226,7 +7232,7 @@
         <xdr:cNvPr id="24" name="Рисунок 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{11736048-5098-4D2E-9E1A-8B5670EA706B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11736048-5098-4D2E-9E1A-8B5670EA706B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7276,7 +7282,7 @@
         <xdr:cNvPr id="44" name="Рисунок 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E3F2769F-B97A-4A9C-B90A-4FE3F0D035C1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3F2769F-B97A-4A9C-B90A-4FE3F0D035C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7326,7 +7332,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{572F6522-EA70-48CF-8A92-E1D9E14FB63D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{572F6522-EA70-48CF-8A92-E1D9E14FB63D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7376,7 +7382,7 @@
         <xdr:cNvPr id="23" name="Рисунок 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9DD18487-6319-4BE8-A07D-E4D469E85F05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DD18487-6319-4BE8-A07D-E4D469E85F05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7431,7 +7437,7 @@
         <xdr:cNvPr id="18" name="Picture 1029">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7505,7 +7511,7 @@
         <xdr:cNvPr id="89" name="Рисунок 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000059000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000059000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7548,7 +7554,7 @@
         <xdr:cNvPr id="90" name="Рисунок 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-00005A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7592,7 +7598,7 @@
         <xdr:cNvPr id="95" name="Рисунок 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-00005F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7636,7 +7642,7 @@
         <xdr:cNvPr id="96" name="Рисунок 95">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000060000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000060000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7680,7 +7686,7 @@
         <xdr:cNvPr id="97" name="Рисунок 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000061000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7723,7 +7729,7 @@
         <xdr:cNvPr id="98" name="Рисунок 97">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000062000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000062000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7766,7 +7772,7 @@
         <xdr:cNvPr id="99" name="Рисунок 98">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000063000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000063000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7810,7 +7816,7 @@
         <xdr:cNvPr id="100" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000064000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000064000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7884,7 +7890,7 @@
         <xdr:cNvPr id="101" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000065000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7958,7 +7964,7 @@
         <xdr:cNvPr id="104" name="Рисунок 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000068000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000068000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8002,7 +8008,7 @@
         <xdr:cNvPr id="105" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000069000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000069000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8077,7 +8083,7 @@
 Ð¾Ð»Ð¾Ð´&quot; Ð² Ð¡Ð°Ð¼Ð°ÑÐµ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-00006E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8136,7 +8142,7 @@
         <xdr:cNvPr id="111" name="Рисунок 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-00006F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8180,7 +8186,7 @@
         <xdr:cNvPr id="116" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000074000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000074000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8254,7 +8260,7 @@
         <xdr:cNvPr id="119" name="Рисунок 24" descr="ÐÐ°ÑÑÐ¸Ð½ÐºÐ¸ Ð¿Ð¾ Ð·Ð°Ð¿ÑÐ¾ÑÑ ÐÐ¾ÑÐ¾Ð½Ð° BFL 2500 ÐÐ¸ÑÑ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000077000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000077000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8328,7 +8334,7 @@
         <xdr:cNvPr id="121" name="Рисунок 24" descr="ÐÐ°ÑÑÐ¸Ð½ÐºÐ¸ Ð¿Ð¾ Ð·Ð°Ð¿ÑÐ¾ÑÑ ÐÐ¾ÑÐ¾Ð½Ð° BFL 2500 ÐÐ¸ÑÑ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000079000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000079000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8402,7 +8408,7 @@
         <xdr:cNvPr id="136" name="Рисунок 135" descr="ÐÐ°ÑÑÐ¸Ð½ÐºÐ¸ Ð¿Ð¾ Ð·Ð°Ð¿ÑÐ¾ÑÑ ÐÑÑÑÐºÐ° ÐÐÐ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000088000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000088000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8461,7 +8467,7 @@
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8658289E-E61A-4B13-A3FC-2163BE572521}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8658289E-E61A-4B13-A3FC-2163BE572521}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8505,7 +8511,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59A68D98-4193-43BE-8F32-48D4BDC840B1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A68D98-4193-43BE-8F32-48D4BDC840B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8913,7 +8919,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R51" sqref="R51"/>
+      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8922,7 +8928,7 @@
     <col min="2" max="2" width="29.85546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" style="21" customWidth="1"/>
     <col min="4" max="4" width="39.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="186" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="185" customWidth="1"/>
     <col min="6" max="6" width="35.140625" style="20" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" style="21" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" style="37" customWidth="1"/>
@@ -8947,21 +8953,21 @@
         <v>5</v>
       </c>
       <c r="E1" s="18"/>
-      <c r="F1" s="185"/>
+      <c r="F1" s="184"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="35"/>
       <c r="J1" s="35"/>
       <c r="K1" s="52"/>
       <c r="L1" s="36"/>
-      <c r="P1" s="218"/>
-      <c r="Q1" s="218"/>
-      <c r="R1" s="218"/>
+      <c r="P1" s="227"/>
+      <c r="Q1" s="227"/>
+      <c r="R1" s="227"/>
       <c r="S1" s="117"/>
       <c r="T1" s="118"/>
-      <c r="V1" s="218"/>
-      <c r="W1" s="218"/>
-      <c r="X1" s="218"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
       <c r="Y1" s="117"/>
       <c r="Z1" s="118"/>
     </row>
@@ -8970,8 +8976,8 @@
       <c r="B2" s="25"/>
       <c r="C2" s="24"/>
       <c r="D2" s="25"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="171"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="170"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
@@ -8983,25 +8989,25 @@
       </c>
       <c r="G3" s="27">
         <f>G56+Бонеты!H28</f>
-        <v>2992182289714.7993</v>
+        <v>9461528416033.1992</v>
       </c>
       <c r="H3" s="38">
         <f>H56+Бонеты!I28</f>
-        <v>58850950355405.609</v>
+        <v>58850972989136.516</v>
       </c>
       <c r="I3" s="38">
         <f>I56+Бонеты!J28</f>
-        <v>706996511.51999998</v>
-      </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="172"/>
+        <v>1784519555.52</v>
+      </c>
+      <c r="N3" s="169"/>
+      <c r="O3" s="171"/>
     </row>
     <row r="4" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28"/>
       <c r="B4" s="30"/>
       <c r="C4" s="29"/>
       <c r="D4" s="116"/>
-      <c r="E4" s="192"/>
+      <c r="E4" s="191"/>
       <c r="F4" s="32" t="s">
         <v>8</v>
       </c>
@@ -9019,10 +9025,10 @@
       </c>
       <c r="J4" s="53"/>
       <c r="K4" s="4"/>
-      <c r="N4" s="170"/>
-      <c r="O4" s="173"/>
-    </row>
-    <row r="5" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="N4" s="169"/>
+      <c r="O4" s="172"/>
+    </row>
+    <row r="5" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="137" t="s">
         <v>10</v>
       </c>
@@ -9035,7 +9041,7 @@
       <c r="D5" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="187" t="s">
+      <c r="E5" s="186" t="s">
         <v>54</v>
       </c>
       <c r="F5" s="139" t="s">
@@ -9056,18 +9062,18 @@
       <c r="K5" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="174"/>
-      <c r="O5" s="171"/>
+      <c r="N5" s="173"/>
+      <c r="O5" s="170"/>
     </row>
     <row r="6" spans="1:26" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="211" t="s">
+      <c r="A6" s="220" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="212"/>
-      <c r="C6" s="212"/>
-      <c r="D6" s="212"/>
-      <c r="E6" s="188"/>
-      <c r="F6" s="198" t="s">
+      <c r="B6" s="221"/>
+      <c r="C6" s="221"/>
+      <c r="D6" s="221"/>
+      <c r="E6" s="187"/>
+      <c r="F6" s="197" t="s">
         <v>189</v>
       </c>
       <c r="G6" s="124"/>
@@ -9077,21 +9083,21 @@
       <c r="K6" s="145"/>
       <c r="N6" s="57"/>
     </row>
-    <row r="7" spans="1:26" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A7" s="146">
         <v>1</v>
       </c>
-      <c r="B7" s="199"/>
-      <c r="C7" s="200" t="s">
+      <c r="B7" s="198"/>
+      <c r="C7" s="199" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="201" t="s">
+      <c r="D7" s="200" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="202">
+      <c r="E7" s="201">
         <v>199927</v>
       </c>
-      <c r="F7" s="203">
+      <c r="F7" s="202">
         <f>E7-E7*4%</f>
         <v>191929.92</v>
       </c>
@@ -9117,21 +9123,21 @@
       <c r="L7" s="22"/>
       <c r="N7" s="65"/>
     </row>
-    <row r="8" spans="1:26" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A8" s="146">
         <v>2</v>
       </c>
-      <c r="B8" s="199"/>
-      <c r="C8" s="200" t="s">
+      <c r="B8" s="198"/>
+      <c r="C8" s="199" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="201" t="s">
+      <c r="D8" s="200" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="202">
+      <c r="E8" s="201">
         <v>218712</v>
       </c>
-      <c r="F8" s="203">
+      <c r="F8" s="202">
         <f>E8-E8*4%</f>
         <v>209963.51999999999</v>
       </c>
@@ -9157,21 +9163,21 @@
       <c r="L8" s="22"/>
       <c r="N8" s="58"/>
     </row>
-    <row r="9" spans="1:26" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A9" s="146">
         <v>3</v>
       </c>
-      <c r="B9" s="199"/>
-      <c r="C9" s="200" t="s">
+      <c r="B9" s="198"/>
+      <c r="C9" s="199" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="201" t="s">
+      <c r="D9" s="200" t="s">
         <v>163</v>
       </c>
-      <c r="E9" s="202">
+      <c r="E9" s="201">
         <v>243067.5</v>
       </c>
-      <c r="F9" s="203">
+      <c r="F9" s="202">
         <f t="shared" ref="F9:F53" si="3">E9-E9*4%</f>
         <v>233344.8</v>
       </c>
@@ -9197,21 +9203,21 @@
       <c r="L9" s="22"/>
       <c r="N9" s="59"/>
     </row>
-    <row r="10" spans="1:26" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A10" s="146">
         <v>4</v>
       </c>
-      <c r="B10" s="199"/>
-      <c r="C10" s="200" t="s">
+      <c r="B10" s="198"/>
+      <c r="C10" s="199" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="201" t="s">
+      <c r="D10" s="200" t="s">
         <v>164</v>
       </c>
-      <c r="E10" s="202">
+      <c r="E10" s="201">
         <v>266545.5</v>
       </c>
-      <c r="F10" s="203">
+      <c r="F10" s="202">
         <f t="shared" si="3"/>
         <v>255883.68</v>
       </c>
@@ -9237,21 +9243,21 @@
       <c r="L10" s="22"/>
       <c r="N10" s="65"/>
     </row>
-    <row r="11" spans="1:26" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A11" s="146">
         <v>5</v>
       </c>
-      <c r="B11" s="199"/>
-      <c r="C11" s="200" t="s">
+      <c r="B11" s="198"/>
+      <c r="C11" s="199" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="201" t="s">
+      <c r="D11" s="200" t="s">
         <v>165</v>
       </c>
-      <c r="E11" s="202">
+      <c r="E11" s="201">
         <v>293949.5</v>
       </c>
-      <c r="F11" s="203">
+      <c r="F11" s="202">
         <f t="shared" si="3"/>
         <v>282191.52</v>
       </c>
@@ -9277,21 +9283,21 @@
       <c r="L11" s="22"/>
       <c r="N11" s="58"/>
     </row>
-    <row r="12" spans="1:26" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A12" s="146">
         <v>6</v>
       </c>
-      <c r="B12" s="199"/>
-      <c r="C12" s="200" t="s">
+      <c r="B12" s="198"/>
+      <c r="C12" s="199" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="201" t="s">
+      <c r="D12" s="200" t="s">
         <v>166</v>
       </c>
-      <c r="E12" s="202">
+      <c r="E12" s="201">
         <v>332793.5</v>
       </c>
-      <c r="F12" s="203">
+      <c r="F12" s="202">
         <f t="shared" si="3"/>
         <v>319481.76</v>
       </c>
@@ -9318,14 +9324,14 @@
       <c r="N12" s="59"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="215" t="s">
+      <c r="A13" s="224" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="216"/>
-      <c r="C13" s="216"/>
-      <c r="D13" s="216"/>
-      <c r="E13" s="217"/>
-      <c r="F13" s="197">
+      <c r="B13" s="225"/>
+      <c r="C13" s="225"/>
+      <c r="D13" s="225"/>
+      <c r="E13" s="226"/>
+      <c r="F13" s="196">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -9336,21 +9342,21 @@
       <c r="K13" s="145"/>
       <c r="L13" s="22"/>
     </row>
-    <row r="14" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="146">
         <v>7</v>
       </c>
-      <c r="B14" s="204"/>
-      <c r="C14" s="205" t="s">
+      <c r="B14" s="203"/>
+      <c r="C14" s="204" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="206" t="s">
+      <c r="D14" s="205" t="s">
         <v>180</v>
       </c>
-      <c r="E14" s="207">
+      <c r="E14" s="206">
         <v>164521.5</v>
       </c>
-      <c r="F14" s="208">
+      <c r="F14" s="207">
         <f>E14-E14*4%</f>
         <v>157940.64000000001</v>
       </c>
@@ -9375,21 +9381,21 @@
       </c>
       <c r="L14" s="22"/>
     </row>
-    <row r="15" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="146">
         <v>8</v>
       </c>
-      <c r="B15" s="204"/>
-      <c r="C15" s="205" t="s">
+      <c r="B15" s="203"/>
+      <c r="C15" s="204" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="206" t="s">
+      <c r="D15" s="205" t="s">
         <v>181</v>
       </c>
-      <c r="E15" s="207">
+      <c r="E15" s="206">
         <v>174460</v>
       </c>
-      <c r="F15" s="208">
+      <c r="F15" s="207">
         <f t="shared" si="3"/>
         <v>167481.60000000001</v>
       </c>
@@ -9414,21 +9420,21 @@
       </c>
       <c r="L15" s="22"/>
     </row>
-    <row r="16" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="146">
         <v>9</v>
       </c>
-      <c r="B16" s="204"/>
-      <c r="C16" s="205" t="s">
+      <c r="B16" s="203"/>
+      <c r="C16" s="204" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="206" t="s">
+      <c r="D16" s="205" t="s">
         <v>182</v>
       </c>
-      <c r="E16" s="207">
+      <c r="E16" s="206">
         <v>192010</v>
       </c>
-      <c r="F16" s="208">
+      <c r="F16" s="207">
         <f t="shared" si="3"/>
         <v>184329.60000000001</v>
       </c>
@@ -9453,21 +9459,21 @@
       </c>
       <c r="L16" s="22"/>
     </row>
-    <row r="17" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="146">
         <v>10</v>
       </c>
-      <c r="B17" s="204"/>
-      <c r="C17" s="205" t="s">
+      <c r="B17" s="203"/>
+      <c r="C17" s="204" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="206" t="s">
+      <c r="D17" s="205" t="s">
         <v>183</v>
       </c>
-      <c r="E17" s="207">
+      <c r="E17" s="206">
         <v>210086.5</v>
       </c>
-      <c r="F17" s="208">
+      <c r="F17" s="207">
         <f t="shared" si="3"/>
         <v>201683.04</v>
       </c>
@@ -9492,21 +9498,21 @@
       </c>
       <c r="L17" s="22"/>
     </row>
-    <row r="18" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="146">
         <v>11</v>
       </c>
-      <c r="B18" s="204"/>
-      <c r="C18" s="205" t="s">
+      <c r="B18" s="203"/>
+      <c r="C18" s="204" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="206" t="s">
+      <c r="D18" s="205" t="s">
         <v>184</v>
       </c>
-      <c r="E18" s="207">
+      <c r="E18" s="206">
         <v>233369.5</v>
       </c>
-      <c r="F18" s="208">
+      <c r="F18" s="207">
         <f t="shared" si="3"/>
         <v>224034.72</v>
       </c>
@@ -9533,17 +9539,17 @@
     </row>
     <row r="19" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="146"/>
-      <c r="B19" s="204"/>
-      <c r="C19" s="205" t="s">
+      <c r="B19" s="203"/>
+      <c r="C19" s="204" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="206" t="s">
+      <c r="D19" s="205" t="s">
         <v>185</v>
       </c>
-      <c r="E19" s="207">
+      <c r="E19" s="206">
         <v>255989.5</v>
       </c>
-      <c r="F19" s="208">
+      <c r="F19" s="207">
         <f t="shared" si="3"/>
         <v>245749.92</v>
       </c>
@@ -9559,7 +9565,7 @@
         <f t="shared" si="2"/>
         <v>15482244.960000001</v>
       </c>
-      <c r="J19" s="183">
+      <c r="J19" s="182">
         <f>0.84*0.7*1.4</f>
         <v>0.82319999999999993</v>
       </c>
@@ -9570,17 +9576,17 @@
     </row>
     <row r="20" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="146"/>
-      <c r="B20" s="204"/>
-      <c r="C20" s="205" t="s">
+      <c r="B20" s="203"/>
+      <c r="C20" s="204" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="206" t="s">
+      <c r="D20" s="205" t="s">
         <v>186</v>
       </c>
-      <c r="E20" s="207">
+      <c r="E20" s="206">
         <v>282314.5</v>
       </c>
-      <c r="F20" s="208">
+      <c r="F20" s="207">
         <f t="shared" si="3"/>
         <v>271021.92</v>
       </c>
@@ -9607,17 +9613,17 @@
     </row>
     <row r="21" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="146"/>
-      <c r="B21" s="204"/>
-      <c r="C21" s="205" t="s">
+      <c r="B21" s="203"/>
+      <c r="C21" s="204" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="206" t="s">
+      <c r="D21" s="205" t="s">
         <v>187</v>
       </c>
-      <c r="E21" s="207">
+      <c r="E21" s="206">
         <v>319631</v>
       </c>
-      <c r="F21" s="208">
+      <c r="F21" s="207">
         <f t="shared" si="3"/>
         <v>306845.76</v>
       </c>
@@ -9642,21 +9648,21 @@
       </c>
       <c r="L21" s="22"/>
     </row>
-    <row r="22" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="146">
         <v>12</v>
       </c>
-      <c r="B22" s="204"/>
-      <c r="C22" s="205" t="s">
+      <c r="B22" s="203"/>
+      <c r="C22" s="204" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="206" t="s">
+      <c r="D22" s="205" t="s">
         <v>188</v>
       </c>
-      <c r="E22" s="207">
+      <c r="E22" s="206">
         <v>361114</v>
       </c>
-      <c r="F22" s="208">
+      <c r="F22" s="207">
         <f t="shared" si="3"/>
         <v>346669.44</v>
       </c>
@@ -9682,14 +9688,14 @@
       <c r="L22" s="22"/>
     </row>
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="176" t="s">
+      <c r="A23" s="175" t="s">
         <v>75</v>
       </c>
       <c r="B23" s="124"/>
       <c r="C23" s="124"/>
       <c r="D23" s="124"/>
-      <c r="E23" s="188"/>
-      <c r="F23" s="197">
+      <c r="E23" s="187"/>
+      <c r="F23" s="196">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -9707,8 +9713,8 @@
       <c r="B24" s="130"/>
       <c r="C24" s="130"/>
       <c r="D24" s="130"/>
-      <c r="E24" s="193"/>
-      <c r="F24" s="197">
+      <c r="E24" s="192"/>
+      <c r="F24" s="196">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -9723,21 +9729,21 @@
       <c r="A25" s="146">
         <v>13</v>
       </c>
-      <c r="B25" s="234"/>
-      <c r="C25" s="235" t="s">
+      <c r="B25" s="210"/>
+      <c r="C25" s="211" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="236" t="s">
+      <c r="D25" s="212" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="237">
+      <c r="E25" s="213">
         <v>213544.5</v>
       </c>
-      <c r="F25" s="210">
+      <c r="F25" s="209">
         <f t="shared" si="3"/>
         <v>205002.72</v>
       </c>
-      <c r="G25" s="209">
+      <c r="G25" s="208">
         <f t="shared" si="0"/>
         <v>43777203341.040001</v>
       </c>
@@ -9758,25 +9764,25 @@
       </c>
       <c r="L25" s="22"/>
     </row>
-    <row r="26" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="146">
         <v>14</v>
       </c>
-      <c r="B26" s="234"/>
-      <c r="C26" s="235" t="s">
+      <c r="B26" s="210"/>
+      <c r="C26" s="211" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="236" t="s">
+      <c r="D26" s="212" t="s">
         <v>168</v>
       </c>
-      <c r="E26" s="237">
+      <c r="E26" s="213">
         <v>229099</v>
       </c>
-      <c r="F26" s="210">
+      <c r="F26" s="209">
         <f>E26-E26*4%</f>
         <v>219935.04</v>
       </c>
-      <c r="G26" s="209">
+      <c r="G26" s="208">
         <f t="shared" si="0"/>
         <v>50386897728.959999</v>
       </c>
@@ -9797,25 +9803,25 @@
       </c>
       <c r="L26" s="22"/>
     </row>
-    <row r="27" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="146">
         <v>15</v>
       </c>
-      <c r="B27" s="234"/>
-      <c r="C27" s="235" t="s">
+      <c r="B27" s="210"/>
+      <c r="C27" s="211" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="236" t="s">
+      <c r="D27" s="212" t="s">
         <v>169</v>
       </c>
-      <c r="E27" s="237">
+      <c r="E27" s="213">
         <v>253942</v>
       </c>
-      <c r="F27" s="210">
+      <c r="F27" s="209">
         <f t="shared" si="3"/>
         <v>243784.32000000001</v>
       </c>
-      <c r="G27" s="209">
+      <c r="G27" s="208">
         <f t="shared" si="0"/>
         <v>61907077789.440002</v>
       </c>
@@ -9836,25 +9842,25 @@
       </c>
       <c r="L27" s="22"/>
     </row>
-    <row r="28" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="146">
         <v>16</v>
       </c>
-      <c r="B28" s="234"/>
-      <c r="C28" s="235" t="s">
+      <c r="B28" s="210"/>
+      <c r="C28" s="211" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="236" t="s">
+      <c r="D28" s="212" t="s">
         <v>170</v>
       </c>
-      <c r="E28" s="237">
+      <c r="E28" s="213">
         <v>279909.5</v>
       </c>
-      <c r="F28" s="210">
+      <c r="F28" s="209">
         <f t="shared" si="3"/>
         <v>268713.12</v>
       </c>
-      <c r="G28" s="209">
+      <c r="G28" s="208">
         <f t="shared" si="0"/>
         <v>75215355062.639999</v>
       </c>
@@ -9875,25 +9881,25 @@
       </c>
       <c r="L28" s="22"/>
     </row>
-    <row r="29" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="146">
         <v>17</v>
       </c>
-      <c r="B29" s="234"/>
-      <c r="C29" s="235" t="s">
+      <c r="B29" s="210"/>
+      <c r="C29" s="211" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="236" t="s">
+      <c r="D29" s="212" t="s">
         <v>171</v>
       </c>
-      <c r="E29" s="237">
+      <c r="E29" s="213">
         <v>318753.5</v>
       </c>
-      <c r="F29" s="210">
+      <c r="F29" s="209">
         <f t="shared" si="3"/>
         <v>306003.36</v>
       </c>
-      <c r="G29" s="209">
+      <c r="G29" s="208">
         <f t="shared" si="0"/>
         <v>97539642011.759995</v>
       </c>
@@ -9914,25 +9920,25 @@
       </c>
       <c r="L29" s="22"/>
     </row>
-    <row r="30" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" s="146">
         <v>18</v>
       </c>
-      <c r="B30" s="234"/>
-      <c r="C30" s="235" t="s">
+      <c r="B30" s="210"/>
+      <c r="C30" s="211" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="236" t="s">
+      <c r="D30" s="212" t="s">
         <v>172</v>
       </c>
-      <c r="E30" s="237">
+      <c r="E30" s="213">
         <v>344025.5</v>
       </c>
-      <c r="F30" s="210">
+      <c r="F30" s="209">
         <f t="shared" si="3"/>
         <v>330264.48</v>
       </c>
-      <c r="G30" s="209">
+      <c r="G30" s="208">
         <f t="shared" si="0"/>
         <v>113619402864.23999</v>
       </c>
@@ -9960,8 +9966,8 @@
       <c r="B31" s="130"/>
       <c r="C31" s="130"/>
       <c r="D31" s="130"/>
-      <c r="E31" s="193"/>
-      <c r="F31" s="197">
+      <c r="E31" s="192"/>
+      <c r="F31" s="196">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -9975,25 +9981,25 @@
       <c r="K31" s="149"/>
       <c r="L31" s="22"/>
     </row>
-    <row r="32" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="146">
         <v>20</v>
       </c>
-      <c r="B32" s="234"/>
-      <c r="C32" s="235" t="s">
+      <c r="B32" s="210"/>
+      <c r="C32" s="211" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="236" t="s">
+      <c r="D32" s="212" t="s">
         <v>152</v>
       </c>
-      <c r="E32" s="237">
+      <c r="E32" s="213">
         <v>221045.5</v>
       </c>
-      <c r="F32" s="210">
+      <c r="F32" s="209">
         <f t="shared" si="3"/>
         <v>212203.68</v>
       </c>
-      <c r="G32" s="209">
+      <c r="G32" s="208">
         <f t="shared" si="0"/>
         <v>46906668547.439995</v>
       </c>
@@ -10014,25 +10020,25 @@
       </c>
       <c r="L32" s="22"/>
     </row>
-    <row r="33" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="146">
         <v>21</v>
       </c>
-      <c r="B33" s="234"/>
-      <c r="C33" s="235" t="s">
+      <c r="B33" s="210"/>
+      <c r="C33" s="211" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="236" t="s">
+      <c r="D33" s="212" t="s">
         <v>173</v>
       </c>
-      <c r="E33" s="237">
+      <c r="E33" s="213">
         <v>255320</v>
       </c>
-      <c r="F33" s="210">
+      <c r="F33" s="209">
         <f t="shared" si="3"/>
         <v>245107.20000000001</v>
       </c>
-      <c r="G33" s="209">
+      <c r="G33" s="208">
         <f t="shared" si="0"/>
         <v>62580770304</v>
       </c>
@@ -10053,25 +10059,25 @@
       </c>
       <c r="L33" s="22"/>
     </row>
-    <row r="34" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="146">
         <v>22</v>
       </c>
-      <c r="B34" s="234"/>
-      <c r="C34" s="235" t="s">
+      <c r="B34" s="210"/>
+      <c r="C34" s="211" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="236" t="s">
+      <c r="D34" s="212" t="s">
         <v>174</v>
       </c>
-      <c r="E34" s="237">
+      <c r="E34" s="213">
         <v>283946</v>
       </c>
-      <c r="F34" s="210">
+      <c r="F34" s="209">
         <f t="shared" si="3"/>
         <v>272588.15999999997</v>
       </c>
-      <c r="G34" s="209">
+      <c r="G34" s="208">
         <f t="shared" si="0"/>
         <v>77400317679.359985</v>
       </c>
@@ -10092,25 +10098,25 @@
       </c>
       <c r="L34" s="22"/>
     </row>
-    <row r="35" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="146">
         <v>23</v>
       </c>
-      <c r="B35" s="234"/>
-      <c r="C35" s="235" t="s">
+      <c r="B35" s="210"/>
+      <c r="C35" s="211" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="236" t="s">
+      <c r="D35" s="212" t="s">
         <v>175</v>
       </c>
-      <c r="E35" s="237">
+      <c r="E35" s="213">
         <v>312403</v>
       </c>
-      <c r="F35" s="210">
+      <c r="F35" s="209">
         <f t="shared" si="3"/>
         <v>299906.88</v>
       </c>
-      <c r="G35" s="209">
+      <c r="G35" s="208">
         <f t="shared" si="0"/>
         <v>93691809032.639999</v>
       </c>
@@ -10131,25 +10137,25 @@
       </c>
       <c r="L35" s="22"/>
     </row>
-    <row r="36" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="146">
         <v>24</v>
       </c>
-      <c r="B36" s="234"/>
-      <c r="C36" s="235" t="s">
+      <c r="B36" s="210"/>
+      <c r="C36" s="211" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="236" t="s">
+      <c r="D36" s="212" t="s">
         <v>176</v>
       </c>
-      <c r="E36" s="237">
+      <c r="E36" s="213">
         <v>340619.5</v>
       </c>
-      <c r="F36" s="210">
+      <c r="F36" s="209">
         <f t="shared" si="3"/>
         <v>326994.71999999997</v>
       </c>
-      <c r="G36" s="209">
+      <c r="G36" s="208">
         <f t="shared" si="0"/>
         <v>111380778029.03999</v>
       </c>
@@ -10170,25 +10176,25 @@
       </c>
       <c r="L36" s="22"/>
     </row>
-    <row r="37" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="146">
         <v>25</v>
       </c>
-      <c r="B37" s="234"/>
-      <c r="C37" s="235" t="s">
+      <c r="B37" s="210"/>
+      <c r="C37" s="211" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="236" t="s">
+      <c r="D37" s="212" t="s">
         <v>177</v>
       </c>
-      <c r="E37" s="237">
+      <c r="E37" s="213">
         <v>386210.5</v>
       </c>
-      <c r="F37" s="210">
+      <c r="F37" s="209">
         <f t="shared" si="3"/>
         <v>370762.08</v>
       </c>
-      <c r="G37" s="209">
+      <c r="G37" s="208">
         <f t="shared" si="0"/>
         <v>143192208297.84</v>
       </c>
@@ -10210,14 +10216,14 @@
       <c r="L37" s="22"/>
     </row>
     <row r="38" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="177" t="s">
+      <c r="A38" s="176" t="s">
         <v>90</v>
       </c>
       <c r="B38" s="132"/>
       <c r="C38" s="132"/>
       <c r="D38" s="132"/>
-      <c r="E38" s="194"/>
-      <c r="F38" s="197">
+      <c r="E38" s="193"/>
+      <c r="F38" s="196">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10232,17 +10238,17 @@
       <c r="A39" s="146">
         <v>26</v>
       </c>
-      <c r="B39" s="238"/>
-      <c r="C39" s="235" t="s">
+      <c r="B39" s="214"/>
+      <c r="C39" s="211" t="s">
         <v>91</v>
       </c>
-      <c r="D39" s="239" t="s">
+      <c r="D39" s="215" t="s">
         <v>140</v>
       </c>
-      <c r="E39" s="237">
+      <c r="E39" s="213">
         <v>169708.5</v>
       </c>
-      <c r="F39" s="210">
+      <c r="F39" s="209">
         <f t="shared" si="3"/>
         <v>162920.16</v>
       </c>
@@ -10271,17 +10277,17 @@
       <c r="A40" s="146">
         <v>27</v>
       </c>
-      <c r="B40" s="238"/>
-      <c r="C40" s="235" t="s">
+      <c r="B40" s="214"/>
+      <c r="C40" s="211" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="239" t="s">
+      <c r="D40" s="215" t="s">
         <v>139</v>
       </c>
-      <c r="E40" s="237">
+      <c r="E40" s="213">
         <v>179965.5</v>
       </c>
-      <c r="F40" s="210">
+      <c r="F40" s="209">
         <f t="shared" si="3"/>
         <v>172766.88</v>
       </c>
@@ -10310,17 +10316,17 @@
       <c r="A41" s="146">
         <v>28</v>
       </c>
-      <c r="B41" s="238"/>
-      <c r="C41" s="235" t="s">
+      <c r="B41" s="214"/>
+      <c r="C41" s="211" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="239" t="s">
+      <c r="D41" s="215" t="s">
         <v>138</v>
       </c>
-      <c r="E41" s="237">
+      <c r="E41" s="213">
         <v>198061.5</v>
       </c>
-      <c r="F41" s="210">
+      <c r="F41" s="209">
         <f t="shared" si="3"/>
         <v>190139.04</v>
       </c>
@@ -10349,17 +10355,17 @@
       <c r="A42" s="146">
         <v>29</v>
       </c>
-      <c r="B42" s="238"/>
-      <c r="C42" s="235" t="s">
+      <c r="B42" s="214"/>
+      <c r="C42" s="211" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="239" t="s">
+      <c r="D42" s="215" t="s">
         <v>141</v>
       </c>
-      <c r="E42" s="237">
+      <c r="E42" s="213">
         <v>216710</v>
       </c>
-      <c r="F42" s="210">
+      <c r="F42" s="209">
         <f>E42-E42*4%</f>
         <v>208041.60000000001</v>
       </c>
@@ -10388,17 +10394,17 @@
       <c r="A43" s="146">
         <v>30</v>
       </c>
-      <c r="B43" s="238"/>
-      <c r="C43" s="235" t="s">
+      <c r="B43" s="214"/>
+      <c r="C43" s="211" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="239" t="s">
+      <c r="D43" s="215" t="s">
         <v>137</v>
       </c>
-      <c r="E43" s="237">
+      <c r="E43" s="213">
         <v>240727.5</v>
       </c>
-      <c r="F43" s="210">
+      <c r="F43" s="209">
         <f t="shared" si="3"/>
         <v>231098.4</v>
       </c>
@@ -10427,17 +10433,17 @@
       <c r="A44" s="146">
         <v>31</v>
       </c>
-      <c r="B44" s="238"/>
-      <c r="C44" s="235" t="s">
+      <c r="B44" s="214"/>
+      <c r="C44" s="211" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="239" t="s">
+      <c r="D44" s="215" t="s">
         <v>136</v>
       </c>
-      <c r="E44" s="237">
+      <c r="E44" s="213">
         <v>264069</v>
       </c>
-      <c r="F44" s="210">
+      <c r="F44" s="209">
         <f t="shared" si="3"/>
         <v>253506.24</v>
       </c>
@@ -10466,17 +10472,17 @@
       <c r="A45" s="146">
         <v>32</v>
       </c>
-      <c r="B45" s="238"/>
-      <c r="C45" s="235" t="s">
+      <c r="B45" s="214"/>
+      <c r="C45" s="211" t="s">
         <v>97</v>
       </c>
-      <c r="D45" s="239" t="s">
+      <c r="D45" s="215" t="s">
         <v>135</v>
       </c>
-      <c r="E45" s="237">
+      <c r="E45" s="213">
         <v>291213</v>
       </c>
-      <c r="F45" s="210">
+      <c r="F45" s="209">
         <f t="shared" si="3"/>
         <v>279564.48</v>
       </c>
@@ -10505,17 +10511,17 @@
       <c r="A46" s="146">
         <v>33</v>
       </c>
-      <c r="B46" s="238"/>
-      <c r="C46" s="235" t="s">
+      <c r="B46" s="214"/>
+      <c r="C46" s="211" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="239" t="s">
+      <c r="D46" s="215" t="s">
         <v>142</v>
       </c>
-      <c r="E46" s="237">
+      <c r="E46" s="213">
         <v>329719</v>
       </c>
-      <c r="F46" s="210">
+      <c r="F46" s="209">
         <f t="shared" si="3"/>
         <v>316530.24</v>
       </c>
@@ -10544,17 +10550,17 @@
       <c r="A47" s="146">
         <v>34</v>
       </c>
-      <c r="B47" s="238"/>
-      <c r="C47" s="235" t="s">
+      <c r="B47" s="214"/>
+      <c r="C47" s="211" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="239" t="s">
+      <c r="D47" s="215" t="s">
         <v>143</v>
       </c>
-      <c r="E47" s="237">
+      <c r="E47" s="213">
         <v>372502</v>
       </c>
-      <c r="F47" s="210">
+      <c r="F47" s="209">
         <f t="shared" si="3"/>
         <v>357601.92</v>
       </c>
@@ -10580,14 +10586,14 @@
       <c r="L47" s="22"/>
     </row>
     <row r="48" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="213" t="s">
+      <c r="A48" s="222" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="214"/>
-      <c r="C48" s="214"/>
-      <c r="D48" s="214"/>
-      <c r="E48" s="190"/>
-      <c r="F48" s="197">
+      <c r="B48" s="223"/>
+      <c r="C48" s="223"/>
+      <c r="D48" s="223"/>
+      <c r="E48" s="189"/>
+      <c r="F48" s="196">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10602,17 +10608,17 @@
       <c r="A49" s="146">
         <v>35</v>
       </c>
-      <c r="B49" s="238"/>
-      <c r="C49" s="235" t="s">
+      <c r="B49" s="214"/>
+      <c r="C49" s="211" t="s">
         <v>101</v>
       </c>
-      <c r="D49" s="239" t="s">
+      <c r="D49" s="215" t="s">
         <v>145</v>
       </c>
-      <c r="E49" s="237">
+      <c r="E49" s="213">
         <v>255866</v>
       </c>
-      <c r="F49" s="210">
+      <c r="F49" s="209">
         <f>E49-E49*4%</f>
         <v>245631.35999999999</v>
       </c>
@@ -10641,17 +10647,17 @@
       <c r="A50" s="146">
         <v>36</v>
       </c>
-      <c r="B50" s="238"/>
-      <c r="C50" s="235" t="s">
+      <c r="B50" s="214"/>
+      <c r="C50" s="211" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="239" t="s">
+      <c r="D50" s="215" t="s">
         <v>144</v>
       </c>
-      <c r="E50" s="237">
+      <c r="E50" s="213">
         <v>278772</v>
       </c>
-      <c r="F50" s="210">
+      <c r="F50" s="209">
         <f t="shared" si="3"/>
         <v>267621.12</v>
       </c>
@@ -10680,17 +10686,17 @@
       <c r="A51" s="146">
         <v>37</v>
       </c>
-      <c r="B51" s="238"/>
-      <c r="C51" s="235" t="s">
+      <c r="B51" s="214"/>
+      <c r="C51" s="211" t="s">
         <v>103</v>
       </c>
-      <c r="D51" s="239" t="s">
+      <c r="D51" s="215" t="s">
         <v>135</v>
       </c>
-      <c r="E51" s="237">
+      <c r="E51" s="213">
         <v>305916</v>
       </c>
-      <c r="F51" s="210">
+      <c r="F51" s="209">
         <f t="shared" si="3"/>
         <v>293679.35999999999</v>
       </c>
@@ -10719,17 +10725,17 @@
       <c r="A52" s="146">
         <v>38</v>
       </c>
-      <c r="B52" s="238"/>
-      <c r="C52" s="235" t="s">
+      <c r="B52" s="214"/>
+      <c r="C52" s="211" t="s">
         <v>104</v>
       </c>
-      <c r="D52" s="239" t="s">
+      <c r="D52" s="215" t="s">
         <v>146</v>
       </c>
-      <c r="E52" s="237">
+      <c r="E52" s="213">
         <v>344422</v>
       </c>
-      <c r="F52" s="210">
+      <c r="F52" s="209">
         <f t="shared" si="3"/>
         <v>330645.12</v>
       </c>
@@ -10758,17 +10764,17 @@
       <c r="A53" s="152">
         <v>39</v>
       </c>
-      <c r="B53" s="240"/>
-      <c r="C53" s="241" t="s">
+      <c r="B53" s="216"/>
+      <c r="C53" s="217" t="s">
         <v>105</v>
       </c>
-      <c r="D53" s="242" t="s">
+      <c r="D53" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="E53" s="243">
+      <c r="E53" s="219">
         <v>387211.5</v>
       </c>
-      <c r="F53" s="210">
+      <c r="F53" s="209">
         <f t="shared" si="3"/>
         <v>371723.04</v>
       </c>
@@ -10804,7 +10810,7 @@
       <c r="D54" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="195" t="e">
+      <c r="E54" s="194" t="e">
         <v>#REF!</v>
       </c>
       <c r="F54" s="123"/>
@@ -10840,7 +10846,7 @@
       <c r="D55" s="110" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="196" t="e">
+      <c r="E55" s="195" t="e">
         <v>#REF!</v>
       </c>
       <c r="F55" s="107"/>
@@ -10867,7 +10873,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D56" s="104"/>
-      <c r="F56" s="168"/>
+      <c r="F56" s="167"/>
       <c r="G56" s="136">
         <f>SUM(G7:G53)</f>
         <v>2992182289714.7993</v>
@@ -10921,19 +10927,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="22" style="21" customWidth="1"/>
     <col min="4" max="4" width="30.140625" style="104" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="186" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="185" customWidth="1"/>
     <col min="7" max="7" width="19" style="20" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" style="21" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" style="37" customWidth="1"/>
@@ -10965,18 +10971,18 @@
         <v>5</v>
       </c>
       <c r="E1" s="18"/>
-      <c r="F1" s="185"/>
+      <c r="F1" s="184"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="35"/>
       <c r="J1" s="35"/>
-      <c r="P1" s="218"/>
-      <c r="Q1" s="218"/>
-      <c r="R1" s="218"/>
+      <c r="P1" s="227"/>
+      <c r="Q1" s="227"/>
+      <c r="R1" s="227"/>
       <c r="S1" s="117"/>
-      <c r="V1" s="218"/>
-      <c r="W1" s="218"/>
-      <c r="X1" s="218"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
       <c r="Y1" s="117"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -11003,15 +11009,15 @@
       </c>
       <c r="H3" s="27">
         <f>H28+Лари!G56</f>
-        <v>2992182289714.7993</v>
+        <v>9461528416033.1992</v>
       </c>
       <c r="I3" s="39">
         <f>I28+Лари!H56</f>
-        <v>58850950355405.609</v>
+        <v>58850972989136.516</v>
       </c>
       <c r="J3" s="39">
         <f>J28+Лари!I56</f>
-        <v>706996511.51999998</v>
+        <v>1784519555.52</v>
       </c>
       <c r="O3" s="16"/>
       <c r="P3" s="57"/>
@@ -11032,15 +11038,15 @@
       </c>
       <c r="H4" s="99">
         <f>H28</f>
-        <v>0</v>
+        <v>6469346126318.4004</v>
       </c>
       <c r="I4" s="39">
         <f>I28</f>
-        <v>0</v>
+        <v>22633730.907839999</v>
       </c>
       <c r="J4" s="39">
         <f>J28</f>
-        <v>0</v>
+        <v>1077523044</v>
       </c>
       <c r="K4" s="53"/>
       <c r="L4" s="4"/>
@@ -11068,7 +11074,7 @@
       <c r="E5" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="187" t="s">
+      <c r="F5" s="186" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="160" t="s">
@@ -11097,15 +11103,15 @@
       <c r="X5" s="64"/>
     </row>
     <row r="6" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="211" t="s">
+      <c r="A6" s="220" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="223"/>
-      <c r="C6" s="223"/>
-      <c r="D6" s="223"/>
-      <c r="E6" s="223"/>
-      <c r="F6" s="188"/>
-      <c r="G6" s="169"/>
+      <c r="B6" s="232"/>
+      <c r="C6" s="232"/>
+      <c r="D6" s="232"/>
+      <c r="E6" s="232"/>
+      <c r="F6" s="187"/>
+      <c r="G6" s="168"/>
       <c r="H6" s="129"/>
       <c r="I6" s="133"/>
       <c r="J6" s="133"/>
@@ -11117,31 +11123,34 @@
       <c r="A7" s="161">
         <v>1</v>
       </c>
-      <c r="B7" s="125"/>
-      <c r="C7" s="178" t="s">
+      <c r="B7" s="243"/>
+      <c r="C7" s="177" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="179" t="s">
+      <c r="D7" s="178" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="175" t="s">
+      <c r="E7" s="174" t="s">
         <v>153</v>
       </c>
-      <c r="F7" s="189">
+      <c r="F7" s="188">
         <v>619242</v>
       </c>
-      <c r="G7" s="157"/>
+      <c r="G7" s="157">
+        <f>F7-F7*4%</f>
+        <v>594472.31999999995</v>
+      </c>
       <c r="H7" s="158">
         <f>F7*G7</f>
-        <v>0</v>
+        <v>368122228381.43994</v>
       </c>
       <c r="I7" s="127">
         <f t="shared" ref="I7:I27" si="0">K7*G7</f>
-        <v>0</v>
+        <v>877441.14431999996</v>
       </c>
       <c r="J7" s="127">
         <f t="shared" ref="J7:J27" si="1">L7*G7</f>
-        <v>0</v>
+        <v>74309040</v>
       </c>
       <c r="K7" s="128">
         <f>0.82*0.9*2</f>
@@ -11156,31 +11165,34 @@
       <c r="A8" s="161">
         <v>2</v>
       </c>
-      <c r="B8" s="125"/>
-      <c r="C8" s="178" t="s">
+      <c r="B8" s="243"/>
+      <c r="C8" s="177" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="179" t="s">
+      <c r="D8" s="178" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="175" t="s">
+      <c r="E8" s="174" t="s">
         <v>154</v>
       </c>
-      <c r="F8" s="189">
+      <c r="F8" s="188">
         <v>689799.5</v>
       </c>
-      <c r="G8" s="157"/>
+      <c r="G8" s="157">
+        <f t="shared" ref="G8:G27" si="2">F8-F8*4%</f>
+        <v>662207.52</v>
+      </c>
       <c r="H8" s="158">
-        <f t="shared" ref="H8:H27" si="2">F8*G8</f>
-        <v>0</v>
+        <f t="shared" ref="H8:H27" si="3">F8*G8</f>
+        <v>456790416192.23999</v>
       </c>
       <c r="I8" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1221772.8744000001</v>
       </c>
       <c r="J8" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>98006712.960000008</v>
       </c>
       <c r="K8" s="128">
         <f>0.82*0.9*2.5</f>
@@ -11192,15 +11204,18 @@
       <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="219" t="s">
+      <c r="A9" s="228" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="220"/>
-      <c r="C9" s="220"/>
-      <c r="D9" s="220"/>
-      <c r="E9" s="220"/>
-      <c r="F9" s="190"/>
-      <c r="G9" s="169"/>
+      <c r="B9" s="229"/>
+      <c r="C9" s="229"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="157">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="H9" s="129"/>
       <c r="I9" s="133"/>
       <c r="J9" s="133"/>
@@ -11212,31 +11227,34 @@
       <c r="A10" s="161">
         <v>3</v>
       </c>
-      <c r="B10" s="125"/>
-      <c r="C10" s="178" t="s">
+      <c r="B10" s="243"/>
+      <c r="C10" s="177" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="179" t="s">
+      <c r="D10" s="178" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="175" t="s">
+      <c r="E10" s="174" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="189">
+      <c r="F10" s="188">
         <v>691099.5</v>
       </c>
-      <c r="G10" s="157"/>
+      <c r="G10" s="157">
+        <f t="shared" si="2"/>
+        <v>663455.52</v>
+      </c>
       <c r="H10" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>458513778144.23999</v>
       </c>
       <c r="I10" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>979260.34752000007</v>
       </c>
       <c r="J10" s="127">
         <f>L10*G10</f>
-        <v>0</v>
+        <v>88903039.680000007</v>
       </c>
       <c r="K10" s="128">
         <f>0.82*0.9*2</f>
@@ -11251,31 +11269,34 @@
       <c r="A11" s="161">
         <v>4</v>
       </c>
-      <c r="B11" s="125"/>
-      <c r="C11" s="178" t="s">
+      <c r="B11" s="243"/>
+      <c r="C11" s="177" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="179" t="s">
+      <c r="D11" s="178" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="175" t="s">
+      <c r="E11" s="174" t="s">
         <v>155</v>
       </c>
-      <c r="F11" s="189">
+      <c r="F11" s="188">
         <v>751016.5</v>
       </c>
-      <c r="G11" s="157"/>
+      <c r="G11" s="157">
+        <f t="shared" si="2"/>
+        <v>720975.84</v>
+      </c>
       <c r="H11" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>541464751941.35999</v>
       </c>
       <c r="I11" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1330200.4247999999</v>
       </c>
       <c r="J11" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>112472231.03999999</v>
       </c>
       <c r="K11" s="128">
         <f>0.82*0.9*2.5</f>
@@ -11287,15 +11308,18 @@
       <c r="M11" s="22"/>
     </row>
     <row r="12" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="219" t="s">
+      <c r="A12" s="228" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="220"/>
-      <c r="C12" s="220"/>
-      <c r="D12" s="220"/>
-      <c r="E12" s="220"/>
-      <c r="F12" s="190"/>
-      <c r="G12" s="169"/>
+      <c r="B12" s="229"/>
+      <c r="C12" s="229"/>
+      <c r="D12" s="229"/>
+      <c r="E12" s="229"/>
+      <c r="F12" s="189"/>
+      <c r="G12" s="157">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="H12" s="129"/>
       <c r="I12" s="133"/>
       <c r="J12" s="133"/>
@@ -11308,30 +11332,33 @@
         <v>5</v>
       </c>
       <c r="B13" s="125"/>
-      <c r="C13" s="178" t="s">
+      <c r="C13" s="177" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="179" t="s">
+      <c r="D13" s="178" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="175" t="s">
+      <c r="E13" s="174" t="s">
         <v>148</v>
       </c>
-      <c r="F13" s="189">
+      <c r="F13" s="188">
         <v>713654.5</v>
       </c>
-      <c r="G13" s="157"/>
+      <c r="G13" s="157">
+        <f t="shared" si="2"/>
+        <v>685108.32</v>
+      </c>
       <c r="H13" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>488930635555.43994</v>
       </c>
       <c r="I13" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>937228.18175999995</v>
       </c>
       <c r="J13" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>70566156.959999993</v>
       </c>
       <c r="K13" s="128">
         <f>0.8*0.9*1.9</f>
@@ -11347,30 +11374,33 @@
         <v>6</v>
       </c>
       <c r="B14" s="125"/>
-      <c r="C14" s="178" t="s">
+      <c r="C14" s="177" t="s">
         <v>116</v>
       </c>
-      <c r="D14" s="179" t="s">
+      <c r="D14" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="180" t="s">
+      <c r="E14" s="179" t="s">
         <v>156</v>
       </c>
-      <c r="F14" s="189">
+      <c r="F14" s="188">
         <v>713654.5</v>
       </c>
-      <c r="G14" s="157"/>
+      <c r="G14" s="157">
+        <f t="shared" si="2"/>
+        <v>685108.32</v>
+      </c>
       <c r="H14" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>488930635555.43994</v>
       </c>
       <c r="I14" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9958049.4311999995</v>
       </c>
       <c r="J14" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>70566156.959999993</v>
       </c>
       <c r="K14" s="128">
         <f>8.5*0.9*1.9</f>
@@ -11386,30 +11416,33 @@
         <v>7</v>
       </c>
       <c r="B15" s="125"/>
-      <c r="C15" s="178" t="s">
+      <c r="C15" s="177" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="179" t="s">
+      <c r="D15" s="178" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="180" t="s">
+      <c r="E15" s="179" t="s">
         <v>157</v>
       </c>
-      <c r="F15" s="189">
+      <c r="F15" s="188">
         <v>735676.5</v>
       </c>
-      <c r="G15" s="157"/>
+      <c r="G15" s="157">
+        <f t="shared" si="2"/>
+        <v>706249.44</v>
+      </c>
       <c r="H15" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>519571116146.15997</v>
       </c>
       <c r="I15" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1134589.72536</v>
       </c>
       <c r="J15" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79806186.719999999</v>
       </c>
       <c r="K15" s="128">
         <f>0.85*0.9*2.1</f>
@@ -11425,30 +11458,33 @@
         <v>8</v>
       </c>
       <c r="B16" s="125"/>
-      <c r="C16" s="178" t="s">
+      <c r="C16" s="177" t="s">
         <v>118</v>
       </c>
-      <c r="D16" s="179" t="s">
+      <c r="D16" s="178" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="175" t="s">
+      <c r="E16" s="174" t="s">
         <v>158</v>
       </c>
-      <c r="F16" s="189">
+      <c r="F16" s="188">
         <v>760454.5</v>
       </c>
-      <c r="G16" s="157"/>
+      <c r="G16" s="157">
+        <f t="shared" si="2"/>
+        <v>730036.32</v>
+      </c>
       <c r="H16" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>555159404707.43994</v>
       </c>
       <c r="I16" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1396194.4620000001</v>
       </c>
       <c r="J16" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>118265883.83999999</v>
       </c>
       <c r="K16" s="128">
         <f>0.85*0.9*2.5</f>
@@ -11460,15 +11496,18 @@
       <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="219" t="s">
+      <c r="A17" s="228" t="s">
         <v>123</v>
       </c>
-      <c r="B17" s="220"/>
-      <c r="C17" s="220"/>
-      <c r="D17" s="220"/>
-      <c r="E17" s="220"/>
-      <c r="F17" s="190"/>
-      <c r="G17" s="169"/>
+      <c r="B17" s="229"/>
+      <c r="C17" s="229"/>
+      <c r="D17" s="229"/>
+      <c r="E17" s="229"/>
+      <c r="F17" s="189"/>
+      <c r="G17" s="157">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="H17" s="129"/>
       <c r="I17" s="133"/>
       <c r="J17" s="133"/>
@@ -11481,30 +11520,33 @@
         <v>9</v>
       </c>
       <c r="B18" s="125"/>
-      <c r="C18" s="178" t="s">
+      <c r="C18" s="177" t="s">
         <v>124</v>
       </c>
-      <c r="D18" s="179" t="s">
+      <c r="D18" s="178" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="180" t="s">
+      <c r="E18" s="179" t="s">
         <v>149</v>
       </c>
-      <c r="F18" s="189">
+      <c r="F18" s="188">
         <v>770770</v>
       </c>
-      <c r="G18" s="157"/>
+      <c r="G18" s="157">
+        <f t="shared" si="2"/>
+        <v>739939.2</v>
+      </c>
       <c r="H18" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>570322937184</v>
       </c>
       <c r="I18" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1012236.8256</v>
       </c>
       <c r="J18" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>76213737.599999994</v>
       </c>
       <c r="K18" s="128">
         <f>0.8*0.9*1.9</f>
@@ -11520,30 +11562,33 @@
         <v>10</v>
       </c>
       <c r="B19" s="125"/>
-      <c r="C19" s="178" t="s">
+      <c r="C19" s="177" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="179" t="s">
+      <c r="D19" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="E19" s="175" t="s">
+      <c r="E19" s="174" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="189">
+      <c r="F19" s="188">
         <v>770770</v>
       </c>
-      <c r="G19" s="157"/>
+      <c r="G19" s="157">
+        <f t="shared" si="2"/>
+        <v>739939.2</v>
+      </c>
       <c r="H19" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>570322937184</v>
       </c>
       <c r="I19" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1075501.6272</v>
       </c>
       <c r="J19" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>76213737.599999994</v>
       </c>
       <c r="K19" s="128">
         <f>0.85*0.9*1.9</f>
@@ -11559,30 +11604,33 @@
         <v>11</v>
       </c>
       <c r="B20" s="125"/>
-      <c r="C20" s="178" t="s">
+      <c r="C20" s="177" t="s">
         <v>126</v>
       </c>
-      <c r="D20" s="179" t="s">
+      <c r="D20" s="178" t="s">
         <v>121</v>
       </c>
-      <c r="E20" s="175" t="s">
+      <c r="E20" s="174" t="s">
         <v>160</v>
       </c>
-      <c r="F20" s="189">
+      <c r="F20" s="188">
         <v>787982</v>
       </c>
-      <c r="G20" s="157"/>
+      <c r="G20" s="157">
+        <f t="shared" si="2"/>
+        <v>756462.72</v>
+      </c>
       <c r="H20" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>596079007031.03992</v>
       </c>
       <c r="I20" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1215257.35968</v>
       </c>
       <c r="J20" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>85480287.359999999</v>
       </c>
       <c r="K20" s="128">
         <f>0.85*0.9*2.1</f>
@@ -11598,30 +11646,33 @@
         <v>12</v>
       </c>
       <c r="B21" s="159"/>
-      <c r="C21" s="178" t="s">
+      <c r="C21" s="177" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="179" t="s">
+      <c r="D21" s="178" t="s">
         <v>122</v>
       </c>
-      <c r="E21" s="175" t="s">
+      <c r="E21" s="174" t="s">
         <v>179</v>
       </c>
-      <c r="F21" s="189">
+      <c r="F21" s="188">
         <v>814814</v>
       </c>
-      <c r="G21" s="157"/>
+      <c r="G21" s="157">
+        <f t="shared" si="2"/>
+        <v>782221.44</v>
+      </c>
       <c r="H21" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>637364980412.15991</v>
       </c>
       <c r="I21" s="127">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1495998.504</v>
       </c>
       <c r="J21" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>126719873.27999999</v>
       </c>
       <c r="K21" s="128">
         <f>0.85*0.9*2.5</f>
@@ -11633,15 +11684,18 @@
       <c r="M21" s="22"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="211" t="s">
+      <c r="A22" s="220" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="223"/>
-      <c r="C22" s="223"/>
-      <c r="D22" s="223"/>
-      <c r="E22" s="223"/>
-      <c r="F22" s="190"/>
-      <c r="G22" s="169"/>
+      <c r="B22" s="232"/>
+      <c r="C22" s="232"/>
+      <c r="D22" s="232"/>
+      <c r="E22" s="232"/>
+      <c r="F22" s="189"/>
+      <c r="G22" s="157">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="H22" s="129"/>
       <c r="I22" s="133"/>
       <c r="J22" s="133"/>
@@ -11654,20 +11708,23 @@
         <v>11</v>
       </c>
       <c r="B23" s="125"/>
-      <c r="C23" s="222" t="s">
+      <c r="C23" s="231" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="222"/>
-      <c r="E23" s="184" t="s">
+      <c r="D23" s="231"/>
+      <c r="E23" s="183" t="s">
         <v>150</v>
       </c>
-      <c r="F23" s="189">
+      <c r="F23" s="188">
         <v>196937</v>
       </c>
-      <c r="G23" s="157"/>
+      <c r="G23" s="157">
+        <f t="shared" si="2"/>
+        <v>189059.52</v>
+      </c>
       <c r="H23" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>37232814690.239998</v>
       </c>
       <c r="I23" s="127">
         <f t="shared" si="0"/>
@@ -11686,20 +11743,23 @@
         <v>12</v>
       </c>
       <c r="B24" s="125"/>
-      <c r="C24" s="222" t="s">
+      <c r="C24" s="231" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="222"/>
-      <c r="E24" s="184" t="s">
+      <c r="D24" s="231"/>
+      <c r="E24" s="183" t="s">
         <v>151</v>
       </c>
-      <c r="F24" s="189">
+      <c r="F24" s="188">
         <v>223262</v>
       </c>
-      <c r="G24" s="157"/>
+      <c r="G24" s="157">
+        <f t="shared" si="2"/>
+        <v>214331.51999999999</v>
+      </c>
       <c r="H24" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>47852083818.239998</v>
       </c>
       <c r="I24" s="127">
         <f t="shared" si="0"/>
@@ -11718,18 +11778,21 @@
         <v>13</v>
       </c>
       <c r="B25" s="125"/>
-      <c r="C25" s="222" t="s">
+      <c r="C25" s="231" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="222"/>
-      <c r="E25" s="181"/>
-      <c r="F25" s="189">
+      <c r="D25" s="231"/>
+      <c r="E25" s="180"/>
+      <c r="F25" s="188">
         <v>202039.5</v>
       </c>
-      <c r="G25" s="157"/>
+      <c r="G25" s="157">
+        <f t="shared" si="2"/>
+        <v>193957.92</v>
+      </c>
       <c r="H25" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>39187161177.840004</v>
       </c>
       <c r="I25" s="127">
         <f t="shared" si="0"/>
@@ -11748,18 +11811,21 @@
         <v>14</v>
       </c>
       <c r="B26" s="125"/>
-      <c r="C26" s="222" t="s">
+      <c r="C26" s="231" t="s">
         <v>132</v>
       </c>
-      <c r="D26" s="222"/>
-      <c r="E26" s="181"/>
-      <c r="F26" s="189">
+      <c r="D26" s="231"/>
+      <c r="E26" s="180"/>
+      <c r="F26" s="188">
         <v>207129</v>
       </c>
-      <c r="G26" s="157"/>
+      <c r="G26" s="157">
+        <f t="shared" si="2"/>
+        <v>198843.84</v>
+      </c>
       <c r="H26" s="158">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>41186325735.360001</v>
       </c>
       <c r="I26" s="127">
         <f t="shared" si="0"/>
@@ -11778,18 +11844,21 @@
         <v>15</v>
       </c>
       <c r="B27" s="163"/>
-      <c r="C27" s="221" t="s">
+      <c r="C27" s="230" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="221"/>
-      <c r="E27" s="182"/>
-      <c r="F27" s="191">
+      <c r="D27" s="230"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="190">
         <v>233441</v>
       </c>
-      <c r="G27" s="164"/>
-      <c r="H27" s="165">
+      <c r="G27" s="157">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>224103.36</v>
+      </c>
+      <c r="H27" s="164">
+        <f t="shared" si="3"/>
+        <v>52314912461.759995</v>
       </c>
       <c r="I27" s="154">
         <f t="shared" si="0"/>
@@ -11804,18 +11873,18 @@
       <c r="M27" s="22"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F28" s="192"/>
-      <c r="H28" s="166">
+      <c r="F28" s="191"/>
+      <c r="H28" s="165">
         <f>SUM(H6:H27)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="167">
+        <v>6469346126318.4004</v>
+      </c>
+      <c r="I28" s="166">
         <f>SUM(I6:I27)</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="167">
+        <v>22633730.907839999</v>
+      </c>
+      <c r="J28" s="166">
         <f>SUM(J6:J27)</f>
-        <v>0</v>
+        <v>1077523044</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -12072,13 +12141,13 @@
       <c r="P10" s="17"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="224" t="s">
+      <c r="A11" s="233" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="225"/>
-      <c r="C11" s="225"/>
-      <c r="D11" s="225"/>
-      <c r="E11" s="225"/>
+      <c r="B11" s="234"/>
+      <c r="C11" s="234"/>
+      <c r="D11" s="234"/>
+      <c r="E11" s="234"/>
       <c r="F11" s="108"/>
       <c r="G11" s="34"/>
       <c r="H11" s="44"/>
@@ -12130,13 +12199,13 @@
       <c r="Q12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="226" t="s">
+      <c r="A13" s="235" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="227"/>
-      <c r="C13" s="227"/>
-      <c r="D13" s="227"/>
-      <c r="E13" s="227"/>
+      <c r="B13" s="236"/>
+      <c r="C13" s="236"/>
+      <c r="D13" s="236"/>
+      <c r="E13" s="236"/>
       <c r="F13" s="115"/>
       <c r="H13" s="44"/>
       <c r="I13" s="41"/>
@@ -12247,7 +12316,7 @@
       <c r="A17" s="81">
         <v>5</v>
       </c>
-      <c r="B17" s="228"/>
+      <c r="B17" s="237"/>
       <c r="C17" s="111" t="s">
         <v>49</v>
       </c>
@@ -12280,7 +12349,7 @@
       <c r="A18" s="81">
         <v>6</v>
       </c>
-      <c r="B18" s="229"/>
+      <c r="B18" s="238"/>
       <c r="C18" s="112" t="s">
         <v>50</v>
       </c>
@@ -12313,7 +12382,7 @@
       <c r="A19" s="81">
         <v>7</v>
       </c>
-      <c r="B19" s="230"/>
+      <c r="B19" s="239"/>
       <c r="C19" s="113" t="s">
         <v>51</v>
       </c>
@@ -12343,13 +12412,13 @@
       <c r="L19" s="42"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="226" t="s">
+      <c r="A20" s="235" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="227"/>
-      <c r="C20" s="227"/>
-      <c r="D20" s="227"/>
-      <c r="E20" s="227"/>
+      <c r="B20" s="236"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
+      <c r="E20" s="236"/>
       <c r="F20" s="115"/>
       <c r="H20" s="44"/>
       <c r="I20" s="41"/>
@@ -12556,13 +12625,13 @@
       <c r="L26" s="42"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="226" t="s">
+      <c r="A27" s="235" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="227"/>
-      <c r="C27" s="227"/>
-      <c r="D27" s="227"/>
-      <c r="E27" s="227"/>
+      <c r="B27" s="236"/>
+      <c r="C27" s="236"/>
+      <c r="D27" s="236"/>
+      <c r="E27" s="236"/>
       <c r="F27" s="115"/>
       <c r="H27" s="44"/>
       <c r="I27" s="41"/>
@@ -12574,7 +12643,7 @@
       <c r="A28" s="78">
         <v>14</v>
       </c>
-      <c r="B28" s="231"/>
+      <c r="B28" s="240"/>
       <c r="C28" s="111" t="s">
         <v>38</v>
       </c>
@@ -12607,7 +12676,7 @@
       <c r="A29" s="78">
         <v>15</v>
       </c>
-      <c r="B29" s="233"/>
+      <c r="B29" s="242"/>
       <c r="C29" s="113" t="s">
         <v>39</v>
       </c>
@@ -12640,7 +12709,7 @@
       <c r="A30" s="78">
         <v>16</v>
       </c>
-      <c r="B30" s="231"/>
+      <c r="B30" s="240"/>
       <c r="C30" s="111" t="s">
         <v>40</v>
       </c>
@@ -12673,7 +12742,7 @@
       <c r="A31" s="78">
         <v>17</v>
       </c>
-      <c r="B31" s="233"/>
+      <c r="B31" s="242"/>
       <c r="C31" s="113" t="s">
         <v>41</v>
       </c>
@@ -12706,7 +12775,7 @@
       <c r="A32" s="78">
         <v>18</v>
       </c>
-      <c r="B32" s="231"/>
+      <c r="B32" s="240"/>
       <c r="C32" s="83" t="s">
         <v>42</v>
       </c>
@@ -12739,7 +12808,7 @@
       <c r="A33" s="78">
         <v>19</v>
       </c>
-      <c r="B33" s="232"/>
+      <c r="B33" s="241"/>
       <c r="C33" s="84" t="s">
         <v>43</v>
       </c>
@@ -12772,7 +12841,7 @@
       <c r="A34" s="78">
         <v>20</v>
       </c>
-      <c r="B34" s="232"/>
+      <c r="B34" s="241"/>
       <c r="C34" s="84" t="s">
         <v>44</v>
       </c>
@@ -12805,7 +12874,7 @@
       <c r="A35" s="78">
         <v>21</v>
       </c>
-      <c r="B35" s="232"/>
+      <c r="B35" s="241"/>
       <c r="C35" s="84" t="s">
         <v>45</v>
       </c>
@@ -12838,7 +12907,7 @@
       <c r="A36" s="78">
         <v>22</v>
       </c>
-      <c r="B36" s="232"/>
+      <c r="B36" s="241"/>
       <c r="C36" s="84" t="s">
         <v>46</v>
       </c>
@@ -12871,7 +12940,7 @@
       <c r="A37" s="78">
         <v>23</v>
       </c>
-      <c r="B37" s="232"/>
+      <c r="B37" s="241"/>
       <c r="C37" s="84" t="s">
         <v>47</v>
       </c>
@@ -12904,7 +12973,7 @@
       <c r="A38" s="78">
         <v>24</v>
       </c>
-      <c r="B38" s="233"/>
+      <c r="B38" s="242"/>
       <c r="C38" s="85" t="s">
         <v>48</v>
       </c>
@@ -12934,13 +13003,13 @@
       <c r="L38" s="42"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="226" t="s">
+      <c r="A39" s="235" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="227"/>
-      <c r="C39" s="227"/>
-      <c r="D39" s="227"/>
-      <c r="E39" s="227"/>
+      <c r="B39" s="236"/>
+      <c r="C39" s="236"/>
+      <c r="D39" s="236"/>
+      <c r="E39" s="236"/>
       <c r="F39" s="115"/>
       <c r="H39" s="44"/>
       <c r="I39" s="41"/>

</xml_diff>

<commit_message>
Commit Auto (Mon Jun  3 17:24:38     2024)
</commit_message>
<xml_diff>
--- a/SoftIce/ice/Фростор 19.04.24.xlsx
+++ b/SoftIce/ice/Фростор 19.04.24.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\OpenServer 5.4.3\domains\TimeForEeexperiments\SoftIce\ice\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9966D901-41DC-4792-9535-C8D19B79CA47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12408" yWindow="2028" windowWidth="10632" windowHeight="10332" tabRatio="654" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12405" yWindow="2025" windowWidth="10635" windowHeight="10335" tabRatio="654" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лари" sheetId="9" r:id="rId1"/>
@@ -2185,7 +2179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -4192,6 +4186,36 @@
     <xf numFmtId="49" fontId="37" fillId="20" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="24" borderId="38" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="24" borderId="38" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="24" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="24" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="67" fillId="16" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4222,6 +4246,12 @@
     <xf numFmtId="0" fontId="36" fillId="16" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="37" fillId="24" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="56" fillId="16" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4255,45 +4285,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="24" borderId="38" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="24" borderId="38" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="30" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="24" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="24" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="24" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="30" fillId="24" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="31">
-    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Акцент1" xfId="2" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Акцент2" xfId="3" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Акцент3" xfId="4" builtinId="37" customBuiltin="1"/>
@@ -4313,10 +4307,10 @@
     <cellStyle name="Название" xfId="18" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Нейтральный" xfId="19" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Обычный_1705о_1_общий прайс Фростор 2014+3.5%" xfId="29" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Обычный_Балки БТ50" xfId="28" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Обычный_новый прайс ЭКО ТУСТ4" xfId="30" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Обычный 2" xfId="20"/>
+    <cellStyle name="Обычный_1705о_1_общий прайс Фростор 2014+3.5%" xfId="29"/>
+    <cellStyle name="Обычный_Балки БТ50" xfId="28"/>
+    <cellStyle name="Обычный_новый прайс ЭКО ТУСТ4" xfId="30"/>
     <cellStyle name="Плохой" xfId="21" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Пояснение" xfId="22" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Примечание" xfId="23" builtinId="10" customBuiltin="1"/>
@@ -4430,7 +4424,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA1ACFBB-3266-4B51-A6C2-4B4B665E041A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AA1ACFBB-3266-4B51-A6C2-4B4B665E041A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4480,7 +4474,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D66AAD1-5BAC-4739-B721-BD89D97D43C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1D66AAD1-5BAC-4739-B721-BD89D97D43C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4530,7 +4524,7 @@
         <xdr:cNvPr id="9" name="Рисунок 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{505DA658-ADC6-4FE4-B792-BB96AD9F6093}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{505DA658-ADC6-4FE4-B792-BB96AD9F6093}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4580,7 +4574,7 @@
         <xdr:cNvPr id="67" name="Рисунок 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E77DE0E3-172F-4595-BE6F-F3CEDB186E65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E77DE0E3-172F-4595-BE6F-F3CEDB186E65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4630,7 +4624,7 @@
         <xdr:cNvPr id="11" name="Рисунок 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79A97C94-FE7C-45A0-B7B8-B036BAB4F3FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79A97C94-FE7C-45A0-B7B8-B036BAB4F3FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4680,7 +4674,7 @@
         <xdr:cNvPr id="13" name="Рисунок 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08E9F54E-76F7-46D1-83A5-B4A81EF2460A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08E9F54E-76F7-46D1-83A5-B4A81EF2460A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4730,7 +4724,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44CA116D-5A8E-41AA-90C2-8CB1A9920212}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{44CA116D-5A8E-41AA-90C2-8CB1A9920212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4780,7 +4774,7 @@
         <xdr:cNvPr id="72" name="Рисунок 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46FBD2BD-0D57-40BD-BFEC-FD7735425613}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{46FBD2BD-0D57-40BD-BFEC-FD7735425613}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4830,7 +4824,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B4C9062-0C12-49F7-90BD-5DDE7288926E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B4C9062-0C12-49F7-90BD-5DDE7288926E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4880,7 +4874,7 @@
         <xdr:cNvPr id="29" name="Рисунок 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4ACADB7-E340-44C6-BC60-B79F691D3F05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4ACADB7-E340-44C6-BC60-B79F691D3F05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4930,7 +4924,7 @@
         <xdr:cNvPr id="31" name="Рисунок 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E193AA-0463-418B-A287-51BDDB233366}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38E193AA-0463-418B-A287-51BDDB233366}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4980,7 +4974,7 @@
         <xdr:cNvPr id="73" name="Рисунок 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6263A97-EA2C-4AFF-8586-A26B64605C34}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D6263A97-EA2C-4AFF-8586-A26B64605C34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5030,7 +5024,7 @@
         <xdr:cNvPr id="45" name="Рисунок 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5365ADE7-524E-4E5F-B716-EB3E2E2A778C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5365ADE7-524E-4E5F-B716-EB3E2E2A778C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5080,7 +5074,7 @@
         <xdr:cNvPr id="74" name="Рисунок 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{506B0900-2101-4BE5-B706-D446268DE6AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{506B0900-2101-4BE5-B706-D446268DE6AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5130,7 +5124,7 @@
         <xdr:cNvPr id="47" name="Рисунок 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17373A6B-76BB-4D04-AF15-68C877857DD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{17373A6B-76BB-4D04-AF15-68C877857DD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5180,7 +5174,7 @@
         <xdr:cNvPr id="49" name="Рисунок 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC85C092-C4D8-486A-BB15-FAD874504601}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CC85C092-C4D8-486A-BB15-FAD874504601}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5230,7 +5224,7 @@
         <xdr:cNvPr id="76" name="Рисунок 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD4298F1-43FE-40C0-ACEA-7D8E8E9B0F37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD4298F1-43FE-40C0-ACEA-7D8E8E9B0F37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5280,7 +5274,7 @@
         <xdr:cNvPr id="78" name="Рисунок 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5305F545-6052-4D32-8FDE-597AAA8618DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5305F545-6052-4D32-8FDE-597AAA8618DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5330,7 +5324,7 @@
         <xdr:cNvPr id="79" name="Рисунок 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{649E095E-F9C8-4240-A2CE-5CB04D065F73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{649E095E-F9C8-4240-A2CE-5CB04D065F73}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5380,7 +5374,7 @@
         <xdr:cNvPr id="81" name="Рисунок 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84E66361-F1C9-48C5-97C5-7989E7256677}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84E66361-F1C9-48C5-97C5-7989E7256677}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5430,7 +5424,7 @@
         <xdr:cNvPr id="82" name="Рисунок 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F33FED6A-AB08-424E-839A-92BBE28467EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F33FED6A-AB08-424E-839A-92BBE28467EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5480,7 +5474,7 @@
         <xdr:cNvPr id="83" name="Рисунок 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2793BF4B-E02F-4B54-B25D-3E971201BF8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2793BF4B-E02F-4B54-B25D-3E971201BF8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5530,7 +5524,7 @@
         <xdr:cNvPr id="86" name="Рисунок 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F6617C-8859-4576-A17A-8F217C4EF54D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D1F6617C-8859-4576-A17A-8F217C4EF54D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5580,7 +5574,7 @@
         <xdr:cNvPr id="88" name="Рисунок 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FC5458D-3083-4153-B36E-BA187DF72AFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4FC5458D-3083-4153-B36E-BA187DF72AFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5630,7 +5624,7 @@
         <xdr:cNvPr id="89" name="Рисунок 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4007AB70-8047-4149-B0FB-4B51136B8E63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4007AB70-8047-4149-B0FB-4B51136B8E63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5680,7 +5674,7 @@
         <xdr:cNvPr id="91" name="Рисунок 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7EAD394-6B87-49D0-AD64-F146DD8F480E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7EAD394-6B87-49D0-AD64-F146DD8F480E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5730,7 +5724,7 @@
         <xdr:cNvPr id="93" name="Рисунок 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55F031BE-AD15-4B72-983B-E5B8128B6A21}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55F031BE-AD15-4B72-983B-E5B8128B6A21}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5780,7 +5774,7 @@
         <xdr:cNvPr id="95" name="Рисунок 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B85DE6AD-C034-4AAC-A74F-1E36B2375F9C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B85DE6AD-C034-4AAC-A74F-1E36B2375F9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5830,7 +5824,7 @@
         <xdr:cNvPr id="96" name="Рисунок 95">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46A156F9-264B-4A3A-8FFD-ABC238E91EC8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{46A156F9-264B-4A3A-8FFD-ABC238E91EC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5880,7 +5874,7 @@
         <xdr:cNvPr id="98" name="Рисунок 97">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31F77DA2-B3BA-48A6-A56C-E97171595A59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31F77DA2-B3BA-48A6-A56C-E97171595A59}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5930,7 +5924,7 @@
         <xdr:cNvPr id="100" name="Рисунок 99">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9ACC027-E330-49E4-95F6-97B8ABBD43D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9ACC027-E330-49E4-95F6-97B8ABBD43D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5980,7 +5974,7 @@
         <xdr:cNvPr id="101" name="Рисунок 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D277B565-53A9-4844-B749-A173258F13A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D277B565-53A9-4844-B749-A173258F13A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6030,7 +6024,7 @@
         <xdr:cNvPr id="102" name="Рисунок 101">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A043CCF-A8C5-4684-AE89-0C3524E76DB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A043CCF-A8C5-4684-AE89-0C3524E76DB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6080,7 +6074,7 @@
         <xdr:cNvPr id="104" name="Рисунок 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D4224A9-2F80-4EB6-B209-C17281907B3E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7D4224A9-2F80-4EB6-B209-C17281907B3E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6130,7 +6124,7 @@
         <xdr:cNvPr id="106" name="Рисунок 105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C01A40-FA55-426C-A175-52B7F6FB6094}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84C01A40-FA55-426C-A175-52B7F6FB6094}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6180,7 +6174,7 @@
         <xdr:cNvPr id="107" name="Рисунок 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D93B6E-243C-4F3B-8C05-EF7F06238827}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61D93B6E-243C-4F3B-8C05-EF7F06238827}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6230,7 +6224,7 @@
         <xdr:cNvPr id="109" name="Рисунок 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E609CDBB-8C12-4549-BEE5-0826E8E4B88E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E609CDBB-8C12-4549-BEE5-0826E8E4B88E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6280,7 +6274,7 @@
         <xdr:cNvPr id="110" name="Рисунок 109">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98CDDAA0-3942-432D-B14E-48EEFF74AE76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{98CDDAA0-3942-432D-B14E-48EEFF74AE76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6330,7 +6324,7 @@
         <xdr:cNvPr id="111" name="Рисунок 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29875149-6284-464F-88D4-9754C07BB095}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29875149-6284-464F-88D4-9754C07BB095}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6380,7 +6374,7 @@
         <xdr:cNvPr id="113" name="Рисунок 112">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A6C9406-B1DE-4862-B9B3-0B828833B5CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2A6C9406-B1DE-4862-B9B3-0B828833B5CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6430,7 +6424,7 @@
         <xdr:cNvPr id="114" name="Рисунок 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A999D5CB-7B5D-43A4-A1A0-CA90C431ABA5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A999D5CB-7B5D-43A4-A1A0-CA90C431ABA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6480,7 +6474,7 @@
         <xdr:cNvPr id="44" name="Picture 1029">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADBEA432-E081-428F-8714-63084FA11034}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ADBEA432-E081-428F-8714-63084FA11034}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6559,7 +6553,7 @@
         <xdr:cNvPr id="2" name="Picture 1029">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6633,7 +6627,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24049225-B489-43B7-BDB7-E9C104CBE58C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24049225-B489-43B7-BDB7-E9C104CBE58C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6683,7 +6677,7 @@
         <xdr:cNvPr id="22" name="Рисунок 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD1F57F-2FB2-41EB-9B4B-A6D25C663FA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DBD1F57F-2FB2-41EB-9B4B-A6D25C663FA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6733,7 +6727,7 @@
         <xdr:cNvPr id="12" name="Рисунок 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9DE3604-5C92-4E44-9D03-6A2370D2D838}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9DE3604-5C92-4E44-9D03-6A2370D2D838}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6783,7 +6777,7 @@
         <xdr:cNvPr id="25" name="Рисунок 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5A47B7-2A7D-4CF2-A9AD-76B1936DA0EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD5A47B7-2A7D-4CF2-A9AD-76B1936DA0EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6833,7 +6827,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D00256DC-24EA-4A3B-B959-66E63D67A33D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D00256DC-24EA-4A3B-B959-66E63D67A33D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6883,7 +6877,7 @@
         <xdr:cNvPr id="29" name="Рисунок 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04126507-E026-4C44-9DF0-B777B39F24C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04126507-E026-4C44-9DF0-B777B39F24C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6933,7 +6927,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07222039-639E-48CE-A508-42EE22195058}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07222039-639E-48CE-A508-42EE22195058}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6983,7 +6977,7 @@
         <xdr:cNvPr id="32" name="Рисунок 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03DC5BCE-DF05-4E02-B799-9BFCD9E339F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{03DC5BCE-DF05-4E02-B799-9BFCD9E339F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7033,7 +7027,7 @@
         <xdr:cNvPr id="33" name="Рисунок 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E588EC-6BB7-40E9-8A02-BB6D75E25CAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{98E588EC-6BB7-40E9-8A02-BB6D75E25CAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7083,7 +7077,7 @@
         <xdr:cNvPr id="34" name="Рисунок 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AFC1F9C-C6C4-4F43-926C-C35E93E87BCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2AFC1F9C-C6C4-4F43-926C-C35E93E87BCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7133,7 +7127,7 @@
         <xdr:cNvPr id="35" name="Рисунок 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84D8FA04-08A8-4568-AA26-420F4782336B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84D8FA04-08A8-4568-AA26-420F4782336B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7183,7 +7177,7 @@
         <xdr:cNvPr id="36" name="Рисунок 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D485DEF-63D2-4A35-8991-9D8BF3E5FA6D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D485DEF-63D2-4A35-8991-9D8BF3E5FA6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7233,7 +7227,7 @@
         <xdr:cNvPr id="21" name="Рисунок 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63FB1715-A81A-49F6-8E5F-0E233DED912D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63FB1715-A81A-49F6-8E5F-0E233DED912D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7283,7 +7277,7 @@
         <xdr:cNvPr id="24" name="Рисунок 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11736048-5098-4D2E-9E1A-8B5670EA706B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{11736048-5098-4D2E-9E1A-8B5670EA706B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7333,7 +7327,7 @@
         <xdr:cNvPr id="44" name="Рисунок 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3F2769F-B97A-4A9C-B90A-4FE3F0D035C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E3F2769F-B97A-4A9C-B90A-4FE3F0D035C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7383,7 +7377,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{572F6522-EA70-48CF-8A92-E1D9E14FB63D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{572F6522-EA70-48CF-8A92-E1D9E14FB63D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7433,7 +7427,7 @@
         <xdr:cNvPr id="23" name="Рисунок 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DD18487-6319-4BE8-A07D-E4D469E85F05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9DD18487-6319-4BE8-A07D-E4D469E85F05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7488,7 +7482,7 @@
         <xdr:cNvPr id="18" name="Picture 1029">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7562,7 +7556,7 @@
         <xdr:cNvPr id="89" name="Рисунок 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000059000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000059000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7605,7 +7599,7 @@
         <xdr:cNvPr id="90" name="Рисунок 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7649,7 +7643,7 @@
         <xdr:cNvPr id="95" name="Рисунок 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-00005F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7693,7 +7687,7 @@
         <xdr:cNvPr id="96" name="Рисунок 95">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000060000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000060000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7737,7 +7731,7 @@
         <xdr:cNvPr id="97" name="Рисунок 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000061000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7780,7 +7774,7 @@
         <xdr:cNvPr id="98" name="Рисунок 97">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000062000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000062000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7823,7 +7817,7 @@
         <xdr:cNvPr id="99" name="Рисунок 98">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000063000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000063000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7867,7 +7861,7 @@
         <xdr:cNvPr id="100" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000064000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000064000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7941,7 +7935,7 @@
         <xdr:cNvPr id="101" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000065000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8015,7 +8009,7 @@
         <xdr:cNvPr id="104" name="Рисунок 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000068000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000068000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8059,7 +8053,7 @@
         <xdr:cNvPr id="105" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000069000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000069000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8134,7 +8128,7 @@
 Ð¾Ð»Ð¾Ð´&quot; Ð² Ð¡Ð°Ð¼Ð°ÑÐµ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-00006E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8193,7 +8187,7 @@
         <xdr:cNvPr id="111" name="Рисунок 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-00006F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8237,7 +8231,7 @@
         <xdr:cNvPr id="116" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000074000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000074000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8311,7 +8305,7 @@
         <xdr:cNvPr id="119" name="Рисунок 24" descr="ÐÐ°ÑÑÐ¸Ð½ÐºÐ¸ Ð¿Ð¾ Ð·Ð°Ð¿ÑÐ¾ÑÑ ÐÐ¾ÑÐ¾Ð½Ð° BFL 2500 ÐÐ¸ÑÑ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000077000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000077000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8385,7 +8379,7 @@
         <xdr:cNvPr id="121" name="Рисунок 24" descr="ÐÐ°ÑÑÐ¸Ð½ÐºÐ¸ Ð¿Ð¾ Ð·Ð°Ð¿ÑÐ¾ÑÑ ÐÐ¾ÑÐ¾Ð½Ð° BFL 2500 ÐÐ¸ÑÑ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000079000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000079000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8459,7 +8453,7 @@
         <xdr:cNvPr id="136" name="Рисунок 135" descr="ÐÐ°ÑÑÐ¸Ð½ÐºÐ¸ Ð¿Ð¾ Ð·Ð°Ð¿ÑÐ¾ÑÑ ÐÑÑÑÐºÐ° ÐÐÐ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000088000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000088000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8518,7 +8512,7 @@
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8658289E-E61A-4B13-A3FC-2163BE572521}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8658289E-E61A-4B13-A3FC-2163BE572521}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8562,7 +8556,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A68D98-4193-43BE-8F32-48D4BDC840B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59A68D98-4193-43BE-8F32-48D4BDC840B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8962,7 +8956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -8973,26 +8967,26 @@
       <selection pane="bottomLeft" activeCell="E51" sqref="D51:E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="39.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" style="175" customWidth="1"/>
-    <col min="6" max="6" width="35.109375" style="20" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="21" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" style="37" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="37" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="175" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="37" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="37" customWidth="1"/>
     <col min="10" max="10" width="10" style="52" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="36" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="7"/>
+    <col min="11" max="11" width="9.140625" style="36" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="7" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -9011,18 +9005,18 @@
       <c r="J1" s="35"/>
       <c r="K1" s="52"/>
       <c r="L1" s="36"/>
-      <c r="P1" s="231"/>
-      <c r="Q1" s="231"/>
-      <c r="R1" s="231"/>
+      <c r="P1" s="241"/>
+      <c r="Q1" s="241"/>
+      <c r="R1" s="241"/>
       <c r="S1" s="117"/>
       <c r="T1" s="118"/>
-      <c r="V1" s="231"/>
-      <c r="W1" s="231"/>
-      <c r="X1" s="231"/>
+      <c r="V1" s="241"/>
+      <c r="W1" s="241"/>
+      <c r="X1" s="241"/>
       <c r="Y1" s="117"/>
       <c r="Z1" s="118"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
       <c r="B2" s="25"/>
       <c r="C2" s="24"/>
@@ -9030,7 +9024,7 @@
       <c r="N2" s="166"/>
       <c r="O2" s="167"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
       <c r="B3" s="25"/>
       <c r="C3" s="24"/>
@@ -9053,7 +9047,7 @@
       <c r="N3" s="166"/>
       <c r="O3" s="168"/>
     </row>
-    <row r="4" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28"/>
       <c r="B4" s="30"/>
       <c r="C4" s="29"/>
@@ -9079,7 +9073,7 @@
       <c r="N4" s="166"/>
       <c r="O4" s="169"/>
     </row>
-    <row r="5" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="136" t="s">
         <v>10</v>
       </c>
@@ -9116,13 +9110,13 @@
       <c r="N5" s="170"/>
       <c r="O5" s="167"/>
     </row>
-    <row r="6" spans="1:26" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="224" t="s">
+    <row r="6" spans="1:26" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="234" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="225"/>
-      <c r="C6" s="225"/>
-      <c r="D6" s="225"/>
+      <c r="B6" s="235"/>
+      <c r="C6" s="235"/>
+      <c r="D6" s="235"/>
       <c r="E6" s="177"/>
       <c r="F6" s="185" t="s">
         <v>189</v>
@@ -9134,7 +9128,7 @@
       <c r="K6" s="144"/>
       <c r="N6" s="57"/>
     </row>
-    <row r="7" spans="1:26" ht="156" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A7" s="145">
         <v>1</v>
       </c>
@@ -9174,7 +9168,7 @@
       <c r="L7" s="22"/>
       <c r="N7" s="65"/>
     </row>
-    <row r="8" spans="1:26" ht="156" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A8" s="145">
         <v>2</v>
       </c>
@@ -9214,7 +9208,7 @@
       <c r="L8" s="22"/>
       <c r="N8" s="58"/>
     </row>
-    <row r="9" spans="1:26" ht="156" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A9" s="145">
         <v>3</v>
       </c>
@@ -9254,7 +9248,7 @@
       <c r="L9" s="22"/>
       <c r="N9" s="59"/>
     </row>
-    <row r="10" spans="1:26" ht="156" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A10" s="145">
         <v>4</v>
       </c>
@@ -9294,7 +9288,7 @@
       <c r="L10" s="22"/>
       <c r="N10" s="65"/>
     </row>
-    <row r="11" spans="1:26" ht="156" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A11" s="145">
         <v>5</v>
       </c>
@@ -9334,7 +9328,7 @@
       <c r="L11" s="22"/>
       <c r="N11" s="58"/>
     </row>
-    <row r="12" spans="1:26" ht="156" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A12" s="145">
         <v>6</v>
       </c>
@@ -9374,14 +9368,14 @@
       <c r="L12" s="22"/>
       <c r="N12" s="59"/>
     </row>
-    <row r="13" spans="1:26" ht="18" x14ac:dyDescent="0.3">
-      <c r="A13" s="228" t="s">
+    <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="238" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="229"/>
-      <c r="C13" s="229"/>
-      <c r="D13" s="229"/>
-      <c r="E13" s="230"/>
+      <c r="B13" s="239"/>
+      <c r="C13" s="239"/>
+      <c r="D13" s="239"/>
+      <c r="E13" s="240"/>
       <c r="F13" s="184">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -9393,7 +9387,7 @@
       <c r="K13" s="144"/>
       <c r="L13" s="22"/>
     </row>
-    <row r="14" spans="1:26" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="145">
         <v>7</v>
       </c>
@@ -9432,7 +9426,7 @@
       </c>
       <c r="L14" s="22"/>
     </row>
-    <row r="15" spans="1:26" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="145">
         <v>8</v>
       </c>
@@ -9471,7 +9465,7 @@
       </c>
       <c r="L15" s="22"/>
     </row>
-    <row r="16" spans="1:26" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="145">
         <v>9</v>
       </c>
@@ -9510,7 +9504,7 @@
       </c>
       <c r="L16" s="22"/>
     </row>
-    <row r="17" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="145">
         <v>10</v>
       </c>
@@ -9549,7 +9543,7 @@
       </c>
       <c r="L17" s="22"/>
     </row>
-    <row r="18" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="145">
         <v>11</v>
       </c>
@@ -9588,7 +9582,7 @@
       </c>
       <c r="L18" s="22"/>
     </row>
-    <row r="19" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="145"/>
       <c r="B19" s="191"/>
       <c r="C19" s="192" t="s">
@@ -9625,7 +9619,7 @@
       </c>
       <c r="L19" s="22"/>
     </row>
-    <row r="20" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="145"/>
       <c r="B20" s="191"/>
       <c r="C20" s="192" t="s">
@@ -9662,7 +9656,7 @@
       </c>
       <c r="L20" s="22"/>
     </row>
-    <row r="21" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="145"/>
       <c r="B21" s="191"/>
       <c r="C21" s="192" t="s">
@@ -9699,7 +9693,7 @@
       </c>
       <c r="L21" s="22"/>
     </row>
-    <row r="22" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="145">
         <v>12</v>
       </c>
@@ -9738,7 +9732,7 @@
       </c>
       <c r="L22" s="22"/>
     </row>
-    <row r="23" spans="1:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="171" t="s">
         <v>75</v>
       </c>
@@ -9757,7 +9751,7 @@
       <c r="K23" s="144"/>
       <c r="L23" s="22"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="147" t="s">
         <v>76</v>
       </c>
@@ -9776,7 +9770,7 @@
       <c r="K24" s="148"/>
       <c r="L24" s="22"/>
     </row>
-    <row r="25" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="145">
         <v>13</v>
       </c>
@@ -9815,7 +9809,7 @@
       </c>
       <c r="L25" s="22"/>
     </row>
-    <row r="26" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="145">
         <v>14</v>
       </c>
@@ -9854,7 +9848,7 @@
       </c>
       <c r="L26" s="22"/>
     </row>
-    <row r="27" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="145">
         <v>15</v>
       </c>
@@ -9893,7 +9887,7 @@
       </c>
       <c r="L27" s="22"/>
     </row>
-    <row r="28" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="145">
         <v>16</v>
       </c>
@@ -9932,7 +9926,7 @@
       </c>
       <c r="L28" s="22"/>
     </row>
-    <row r="29" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="145">
         <v>17</v>
       </c>
@@ -9971,7 +9965,7 @@
       </c>
       <c r="L29" s="22"/>
     </row>
-    <row r="30" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" s="145">
         <v>18</v>
       </c>
@@ -10010,7 +10004,7 @@
       </c>
       <c r="L30" s="22"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="147" t="s">
         <v>83</v>
       </c>
@@ -10032,7 +10026,7 @@
       <c r="K31" s="148"/>
       <c r="L31" s="22"/>
     </row>
-    <row r="32" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="145">
         <v>20</v>
       </c>
@@ -10071,7 +10065,7 @@
       </c>
       <c r="L32" s="22"/>
     </row>
-    <row r="33" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="145">
         <v>21</v>
       </c>
@@ -10110,7 +10104,7 @@
       </c>
       <c r="L33" s="22"/>
     </row>
-    <row r="34" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="145">
         <v>22</v>
       </c>
@@ -10149,7 +10143,7 @@
       </c>
       <c r="L34" s="22"/>
     </row>
-    <row r="35" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="145">
         <v>23</v>
       </c>
@@ -10188,7 +10182,7 @@
       </c>
       <c r="L35" s="22"/>
     </row>
-    <row r="36" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="145">
         <v>24</v>
       </c>
@@ -10227,7 +10221,7 @@
       </c>
       <c r="L36" s="22"/>
     </row>
-    <row r="37" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="145">
         <v>25</v>
       </c>
@@ -10266,7 +10260,7 @@
       </c>
       <c r="L37" s="22"/>
     </row>
-    <row r="38" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="172" t="s">
         <v>90</v>
       </c>
@@ -10285,7 +10279,7 @@
       <c r="K38" s="149"/>
       <c r="L38" s="22"/>
     </row>
-    <row r="39" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="145">
         <v>26</v>
       </c>
@@ -10324,7 +10318,7 @@
       </c>
       <c r="L39" s="22"/>
     </row>
-    <row r="40" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="145">
         <v>27</v>
       </c>
@@ -10363,7 +10357,7 @@
       </c>
       <c r="L40" s="22"/>
     </row>
-    <row r="41" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="145">
         <v>28</v>
       </c>
@@ -10387,7 +10381,7 @@
       </c>
       <c r="H41" s="126">
         <f t="shared" si="7"/>
-        <v>1663031308477.5938</v>
+        <v>1663031308477.5937</v>
       </c>
       <c r="I41" s="126">
         <f t="shared" si="8"/>
@@ -10402,7 +10396,7 @@
       </c>
       <c r="L41" s="22"/>
     </row>
-    <row r="42" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="145">
         <v>29</v>
       </c>
@@ -10441,7 +10435,7 @@
       </c>
       <c r="L42" s="22"/>
     </row>
-    <row r="43" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="145">
         <v>30</v>
       </c>
@@ -10480,7 +10474,7 @@
       </c>
       <c r="L43" s="22"/>
     </row>
-    <row r="44" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="145">
         <v>31</v>
       </c>
@@ -10519,7 +10513,7 @@
       </c>
       <c r="L44" s="22"/>
     </row>
-    <row r="45" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="145">
         <v>32</v>
       </c>
@@ -10558,7 +10552,7 @@
       </c>
       <c r="L45" s="22"/>
     </row>
-    <row r="46" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="145">
         <v>33</v>
       </c>
@@ -10597,7 +10591,7 @@
       </c>
       <c r="L46" s="22"/>
     </row>
-    <row r="47" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="145">
         <v>34</v>
       </c>
@@ -10636,13 +10630,13 @@
       </c>
       <c r="L47" s="22"/>
     </row>
-    <row r="48" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="226" t="s">
+    <row r="48" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="236" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="227"/>
-      <c r="C48" s="227"/>
-      <c r="D48" s="227"/>
+      <c r="B48" s="237"/>
+      <c r="C48" s="237"/>
+      <c r="D48" s="237"/>
       <c r="E48" s="178"/>
       <c r="F48" s="184">
         <f t="shared" si="3"/>
@@ -10655,7 +10649,7 @@
       <c r="K48" s="150"/>
       <c r="L48" s="22"/>
     </row>
-    <row r="49" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="145">
         <v>35</v>
       </c>
@@ -10694,7 +10688,7 @@
       </c>
       <c r="L49" s="22"/>
     </row>
-    <row r="50" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="145">
         <v>36</v>
       </c>
@@ -10733,7 +10727,7 @@
       </c>
       <c r="L50" s="22"/>
     </row>
-    <row r="51" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="145">
         <v>37</v>
       </c>
@@ -10772,7 +10766,7 @@
       </c>
       <c r="L51" s="22"/>
     </row>
-    <row r="52" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="145">
         <v>38</v>
       </c>
@@ -10811,7 +10805,7 @@
       </c>
       <c r="L52" s="22"/>
     </row>
-    <row r="53" spans="1:12" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="151">
         <v>39</v>
       </c>
@@ -10850,7 +10844,7 @@
       </c>
       <c r="L53" s="22"/>
     </row>
-    <row r="54" spans="1:12" ht="75.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" ht="75.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="119">
         <v>30</v>
       </c>
@@ -10886,7 +10880,7 @@
       </c>
       <c r="L54" s="22"/>
     </row>
-    <row r="55" spans="1:12" ht="70.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="70.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="105">
         <v>31</v>
       </c>
@@ -10922,7 +10916,7 @@
       </c>
       <c r="L55" s="22"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D56" s="104"/>
       <c r="F56" s="164"/>
       <c r="G56" s="135">
@@ -10941,22 +10935,22 @@
       <c r="K56" s="7"/>
       <c r="L56" s="22"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L57" s="22"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L58" s="22"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L59" s="22"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L60" s="22"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L61" s="22"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L62" s="22"/>
     </row>
   </sheetData>
@@ -10975,42 +10969,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="46" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="C25:G27"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="22" style="21" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="104" customWidth="1"/>
-    <col min="5" max="5" width="40.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="4.109375" style="175" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="104" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="175" customWidth="1"/>
     <col min="7" max="7" width="19" style="20" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="21" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" style="37" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="37" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="21" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="37" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="37" customWidth="1"/>
     <col min="11" max="11" width="10" style="52" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="36"/>
-    <col min="13" max="13" width="12.44140625" style="7" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="7"/>
-    <col min="15" max="15" width="10.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.88671875" style="118" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" style="118" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="9.109375" style="118"/>
-    <col min="21" max="21" width="9.109375" style="7"/>
-    <col min="22" max="22" width="10.88671875" style="118" customWidth="1"/>
-    <col min="23" max="23" width="12.44140625" style="118" customWidth="1"/>
-    <col min="24" max="26" width="9.109375" style="118"/>
-    <col min="27" max="16384" width="9.109375" style="7"/>
+    <col min="12" max="12" width="9.140625" style="36"/>
+    <col min="13" max="13" width="12.42578125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="7"/>
+    <col min="15" max="15" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" style="118" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="118" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="9.140625" style="118"/>
+    <col min="21" max="21" width="9.140625" style="7"/>
+    <col min="22" max="22" width="10.85546875" style="118" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" style="118" customWidth="1"/>
+    <col min="24" max="26" width="9.140625" style="118"/>
+    <col min="27" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -11027,16 +11021,16 @@
       <c r="H1" s="46"/>
       <c r="I1" s="35"/>
       <c r="J1" s="35"/>
-      <c r="P1" s="231"/>
-      <c r="Q1" s="231"/>
-      <c r="R1" s="231"/>
+      <c r="P1" s="241"/>
+      <c r="Q1" s="241"/>
+      <c r="R1" s="241"/>
       <c r="S1" s="117"/>
-      <c r="V1" s="231"/>
-      <c r="W1" s="231"/>
-      <c r="X1" s="231"/>
+      <c r="V1" s="241"/>
+      <c r="W1" s="241"/>
+      <c r="X1" s="241"/>
       <c r="Y1" s="117"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="95"/>
       <c r="B2" s="96"/>
       <c r="C2" s="97"/>
@@ -11049,7 +11043,7 @@
       <c r="W2" s="58"/>
       <c r="X2" s="57"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="95"/>
       <c r="B3" s="96"/>
       <c r="C3" s="97"/>
@@ -11078,7 +11072,7 @@
       <c r="W3" s="60"/>
       <c r="X3" s="61"/>
     </row>
-    <row r="4" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28"/>
       <c r="B4" s="30"/>
       <c r="C4" s="29"/>
@@ -11109,7 +11103,7 @@
       <c r="W4" s="62"/>
       <c r="X4" s="63"/>
     </row>
-    <row r="5" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="136" t="s">
         <v>10</v>
       </c>
@@ -11153,14 +11147,14 @@
       <c r="W5" s="64"/>
       <c r="X5" s="64"/>
     </row>
-    <row r="6" spans="1:25" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="224" t="s">
+    <row r="6" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="234" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="234"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
+      <c r="B6" s="246"/>
+      <c r="C6" s="246"/>
+      <c r="D6" s="246"/>
+      <c r="E6" s="246"/>
       <c r="F6" s="177"/>
       <c r="G6" s="165"/>
       <c r="H6" s="128"/>
@@ -11170,24 +11164,24 @@
       <c r="L6" s="150"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:25" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A7" s="159">
         <v>1</v>
       </c>
       <c r="B7" s="208"/>
-      <c r="C7" s="245" t="s">
+      <c r="C7" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="246" t="s">
+      <c r="D7" s="225" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="247" t="s">
+      <c r="E7" s="226" t="s">
         <v>153</v>
       </c>
-      <c r="F7" s="248">
+      <c r="F7" s="227">
         <v>619242</v>
       </c>
-      <c r="G7" s="249">
+      <c r="G7" s="228">
         <f>F7-F7*4%</f>
         <v>594472.31999999995</v>
       </c>
@@ -11212,24 +11206,24 @@
       </c>
       <c r="M7" s="22"/>
     </row>
-    <row r="8" spans="1:25" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A8" s="159">
         <v>2</v>
       </c>
       <c r="B8" s="208"/>
-      <c r="C8" s="245" t="s">
+      <c r="C8" s="224" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="246" t="s">
+      <c r="D8" s="225" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="247" t="s">
+      <c r="E8" s="226" t="s">
         <v>154</v>
       </c>
-      <c r="F8" s="248">
+      <c r="F8" s="227">
         <v>689799.5</v>
       </c>
-      <c r="G8" s="249">
+      <c r="G8" s="228">
         <f t="shared" ref="G8:G27" si="2">F8-F8*4%</f>
         <v>662207.52</v>
       </c>
@@ -11254,14 +11248,14 @@
       </c>
       <c r="M8" s="22"/>
     </row>
-    <row r="9" spans="1:25" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="232" t="s">
+    <row r="9" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="242" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
+      <c r="B9" s="243"/>
+      <c r="C9" s="243"/>
+      <c r="D9" s="243"/>
+      <c r="E9" s="243"/>
       <c r="F9" s="178"/>
       <c r="G9" s="156">
         <f t="shared" si="2"/>
@@ -11274,24 +11268,24 @@
       <c r="L9" s="150"/>
       <c r="M9" s="22"/>
     </row>
-    <row r="10" spans="1:25" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A10" s="159">
         <v>3</v>
       </c>
       <c r="B10" s="208"/>
-      <c r="C10" s="245" t="s">
+      <c r="C10" s="224" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="246" t="s">
+      <c r="D10" s="225" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="247" t="s">
+      <c r="E10" s="226" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="248">
+      <c r="F10" s="227">
         <v>691099.5</v>
       </c>
-      <c r="G10" s="249">
+      <c r="G10" s="228">
         <f t="shared" si="2"/>
         <v>663455.52</v>
       </c>
@@ -11316,24 +11310,24 @@
       </c>
       <c r="M10" s="22"/>
     </row>
-    <row r="11" spans="1:25" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A11" s="159">
         <v>4</v>
       </c>
       <c r="B11" s="208"/>
-      <c r="C11" s="245" t="s">
+      <c r="C11" s="224" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="246" t="s">
+      <c r="D11" s="225" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="247" t="s">
+      <c r="E11" s="226" t="s">
         <v>155</v>
       </c>
-      <c r="F11" s="248">
+      <c r="F11" s="227">
         <v>751016.5</v>
       </c>
-      <c r="G11" s="249">
+      <c r="G11" s="228">
         <f t="shared" si="2"/>
         <v>720975.84</v>
       </c>
@@ -11358,14 +11352,14 @@
       </c>
       <c r="M11" s="22"/>
     </row>
-    <row r="12" spans="1:25" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="232" t="s">
+    <row r="12" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="242" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="233"/>
-      <c r="C12" s="233"/>
-      <c r="D12" s="233"/>
-      <c r="E12" s="233"/>
+      <c r="B12" s="243"/>
+      <c r="C12" s="243"/>
+      <c r="D12" s="243"/>
+      <c r="E12" s="243"/>
       <c r="F12" s="178"/>
       <c r="G12" s="156">
         <f t="shared" si="2"/>
@@ -11378,7 +11372,7 @@
       <c r="L12" s="150"/>
       <c r="M12" s="22"/>
     </row>
-    <row r="13" spans="1:25" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A13" s="210">
         <v>5</v>
       </c>
@@ -11420,24 +11414,24 @@
       </c>
       <c r="M13" s="22"/>
     </row>
-    <row r="14" spans="1:25" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="159">
         <v>6</v>
       </c>
       <c r="B14" s="209"/>
-      <c r="C14" s="245" t="s">
+      <c r="C14" s="224" t="s">
         <v>116</v>
       </c>
-      <c r="D14" s="246" t="s">
+      <c r="D14" s="225" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="250" t="s">
+      <c r="E14" s="229" t="s">
         <v>156</v>
       </c>
-      <c r="F14" s="248">
+      <c r="F14" s="227">
         <v>713654.5</v>
       </c>
-      <c r="G14" s="249">
+      <c r="G14" s="228">
         <f t="shared" si="2"/>
         <v>685108.32</v>
       </c>
@@ -11462,24 +11456,24 @@
       </c>
       <c r="M14" s="22"/>
     </row>
-    <row r="15" spans="1:25" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="159">
         <v>7</v>
       </c>
       <c r="B15" s="209"/>
-      <c r="C15" s="245" t="s">
+      <c r="C15" s="224" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="246" t="s">
+      <c r="D15" s="225" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="250" t="s">
+      <c r="E15" s="229" t="s">
         <v>157</v>
       </c>
-      <c r="F15" s="248">
+      <c r="F15" s="227">
         <v>735676.5</v>
       </c>
-      <c r="G15" s="249">
+      <c r="G15" s="228">
         <f t="shared" si="2"/>
         <v>706249.44</v>
       </c>
@@ -11504,24 +11498,24 @@
       </c>
       <c r="M15" s="22"/>
     </row>
-    <row r="16" spans="1:25" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A16" s="159">
         <v>8</v>
       </c>
       <c r="B16" s="209"/>
-      <c r="C16" s="245" t="s">
+      <c r="C16" s="224" t="s">
         <v>118</v>
       </c>
-      <c r="D16" s="246" t="s">
+      <c r="D16" s="225" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="247" t="s">
+      <c r="E16" s="226" t="s">
         <v>158</v>
       </c>
-      <c r="F16" s="248">
+      <c r="F16" s="227">
         <v>760454.5</v>
       </c>
-      <c r="G16" s="249">
+      <c r="G16" s="228">
         <f t="shared" si="2"/>
         <v>730036.32</v>
       </c>
@@ -11546,14 +11540,14 @@
       </c>
       <c r="M16" s="22"/>
     </row>
-    <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="232" t="s">
+    <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="242" t="s">
         <v>123</v>
       </c>
-      <c r="B17" s="233"/>
-      <c r="C17" s="233"/>
-      <c r="D17" s="233"/>
-      <c r="E17" s="233"/>
+      <c r="B17" s="243"/>
+      <c r="C17" s="243"/>
+      <c r="D17" s="243"/>
+      <c r="E17" s="243"/>
       <c r="F17" s="178"/>
       <c r="G17" s="156">
         <f t="shared" si="2"/>
@@ -11566,7 +11560,7 @@
       <c r="L17" s="150"/>
       <c r="M17" s="22"/>
     </row>
-    <row r="18" spans="1:13" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="210">
         <v>9</v>
       </c>
@@ -11608,24 +11602,24 @@
       </c>
       <c r="M18" s="22"/>
     </row>
-    <row r="19" spans="1:13" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A19" s="159">
         <v>10</v>
       </c>
       <c r="B19" s="209"/>
-      <c r="C19" s="245" t="s">
+      <c r="C19" s="224" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="246" t="s">
+      <c r="D19" s="225" t="s">
         <v>120</v>
       </c>
-      <c r="E19" s="247" t="s">
+      <c r="E19" s="226" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="248">
+      <c r="F19" s="227">
         <v>770770</v>
       </c>
-      <c r="G19" s="249">
+      <c r="G19" s="228">
         <f t="shared" si="2"/>
         <v>739939.2</v>
       </c>
@@ -11650,24 +11644,24 @@
       </c>
       <c r="M19" s="22"/>
     </row>
-    <row r="20" spans="1:13" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A20" s="159">
         <v>11</v>
       </c>
       <c r="B20" s="209"/>
-      <c r="C20" s="245" t="s">
+      <c r="C20" s="224" t="s">
         <v>126</v>
       </c>
-      <c r="D20" s="246" t="s">
+      <c r="D20" s="225" t="s">
         <v>121</v>
       </c>
-      <c r="E20" s="247" t="s">
+      <c r="E20" s="226" t="s">
         <v>160</v>
       </c>
-      <c r="F20" s="248">
+      <c r="F20" s="227">
         <v>787982</v>
       </c>
-      <c r="G20" s="249">
+      <c r="G20" s="228">
         <f t="shared" si="2"/>
         <v>756462.72</v>
       </c>
@@ -11692,24 +11686,24 @@
       </c>
       <c r="M20" s="22"/>
     </row>
-    <row r="21" spans="1:13" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A21" s="159">
         <v>12</v>
       </c>
       <c r="B21" s="222"/>
-      <c r="C21" s="245" t="s">
+      <c r="C21" s="224" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="246" t="s">
+      <c r="D21" s="225" t="s">
         <v>122</v>
       </c>
-      <c r="E21" s="247" t="s">
+      <c r="E21" s="226" t="s">
         <v>179</v>
       </c>
-      <c r="F21" s="248">
+      <c r="F21" s="227">
         <v>814814</v>
       </c>
-      <c r="G21" s="249">
+      <c r="G21" s="228">
         <f t="shared" si="2"/>
         <v>782221.44</v>
       </c>
@@ -11734,14 +11728,14 @@
       </c>
       <c r="M21" s="22"/>
     </row>
-    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A22" s="224" t="s">
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="234" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="234"/>
-      <c r="C22" s="234"/>
-      <c r="D22" s="234"/>
-      <c r="E22" s="234"/>
+      <c r="B22" s="246"/>
+      <c r="C22" s="246"/>
+      <c r="D22" s="246"/>
+      <c r="E22" s="246"/>
       <c r="F22" s="178"/>
       <c r="G22" s="156">
         <f t="shared" si="2"/>
@@ -11754,22 +11748,22 @@
       <c r="L22" s="150"/>
       <c r="M22" s="22"/>
     </row>
-    <row r="23" spans="1:13" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A23" s="159">
         <v>11</v>
       </c>
       <c r="B23" s="209"/>
-      <c r="C23" s="251" t="s">
+      <c r="C23" s="245" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="251"/>
-      <c r="E23" s="252" t="s">
+      <c r="D23" s="245"/>
+      <c r="E23" s="230" t="s">
         <v>150</v>
       </c>
-      <c r="F23" s="248">
+      <c r="F23" s="227">
         <v>196937</v>
       </c>
-      <c r="G23" s="249">
+      <c r="G23" s="228">
         <f t="shared" si="2"/>
         <v>189059.52</v>
       </c>
@@ -11789,22 +11783,22 @@
       <c r="L23" s="146"/>
       <c r="M23" s="22"/>
     </row>
-    <row r="24" spans="1:13" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A24" s="159">
         <v>12</v>
       </c>
       <c r="B24" s="209"/>
-      <c r="C24" s="251" t="s">
+      <c r="C24" s="245" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="251"/>
-      <c r="E24" s="252" t="s">
+      <c r="D24" s="245"/>
+      <c r="E24" s="230" t="s">
         <v>151</v>
       </c>
-      <c r="F24" s="248">
+      <c r="F24" s="227">
         <v>223262</v>
       </c>
-      <c r="G24" s="249">
+      <c r="G24" s="228">
         <f t="shared" si="2"/>
         <v>214331.51999999999</v>
       </c>
@@ -11824,20 +11818,20 @@
       <c r="L24" s="146"/>
       <c r="M24" s="22"/>
     </row>
-    <row r="25" spans="1:13" ht="110.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="159">
         <v>13</v>
       </c>
       <c r="B25" s="209"/>
-      <c r="C25" s="251" t="s">
+      <c r="C25" s="245" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="251"/>
-      <c r="E25" s="253"/>
-      <c r="F25" s="248">
+      <c r="D25" s="245"/>
+      <c r="E25" s="231"/>
+      <c r="F25" s="227">
         <v>202039.5</v>
       </c>
-      <c r="G25" s="249">
+      <c r="G25" s="228">
         <f t="shared" si="2"/>
         <v>193957.92</v>
       </c>
@@ -11857,20 +11851,20 @@
       <c r="L25" s="146"/>
       <c r="M25" s="22"/>
     </row>
-    <row r="26" spans="1:13" ht="110.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="159">
         <v>14</v>
       </c>
       <c r="B26" s="209"/>
-      <c r="C26" s="251" t="s">
+      <c r="C26" s="245" t="s">
         <v>132</v>
       </c>
-      <c r="D26" s="251"/>
-      <c r="E26" s="253"/>
-      <c r="F26" s="248">
+      <c r="D26" s="245"/>
+      <c r="E26" s="231"/>
+      <c r="F26" s="227">
         <v>207129</v>
       </c>
-      <c r="G26" s="249">
+      <c r="G26" s="228">
         <f t="shared" si="2"/>
         <v>198843.84</v>
       </c>
@@ -11890,20 +11884,20 @@
       <c r="L26" s="146"/>
       <c r="M26" s="22"/>
     </row>
-    <row r="27" spans="1:13" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="160">
         <v>15</v>
       </c>
       <c r="B27" s="223"/>
-      <c r="C27" s="254" t="s">
+      <c r="C27" s="244" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="254"/>
-      <c r="E27" s="255"/>
-      <c r="F27" s="256">
+      <c r="D27" s="244"/>
+      <c r="E27" s="232"/>
+      <c r="F27" s="233">
         <v>233441</v>
       </c>
-      <c r="G27" s="249">
+      <c r="G27" s="228">
         <f t="shared" si="2"/>
         <v>224103.36</v>
       </c>
@@ -11923,7 +11917,7 @@
       <c r="L27" s="155"/>
       <c r="M27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F28" s="179"/>
       <c r="H28" s="162">
         <f>SUM(H6:H27)</f>
@@ -11938,7 +11932,7 @@
         <v>1077523044</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="22"/>
@@ -11966,7 +11960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -11977,29 +11971,29 @@
       <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="20" customWidth="1"/>
     <col min="2" max="2" width="30" style="21" customWidth="1"/>
     <col min="3" max="3" width="54" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="49" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="22" customWidth="1"/>
     <col min="7" max="7" width="19" style="20" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="21" customWidth="1"/>
-    <col min="9" max="10" width="18.5546875" style="37" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="21" customWidth="1"/>
+    <col min="9" max="10" width="18.5703125" style="37" customWidth="1"/>
     <col min="11" max="11" width="10" style="52" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="36" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" style="7" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="7"/>
-    <col min="15" max="15" width="11.33203125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="35.44140625" style="7" customWidth="1"/>
-    <col min="18" max="19" width="10.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.109375" style="7"/>
+    <col min="12" max="12" width="9.140625" style="36" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="7"/>
+    <col min="15" max="15" width="11.28515625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="35.42578125" style="7" customWidth="1"/>
+    <col min="18" max="19" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -12016,7 +12010,7 @@
       <c r="P1" s="10"/>
       <c r="Q1" s="11"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -12033,7 +12027,7 @@
       <c r="P2" s="12"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -12050,7 +12044,7 @@
       <c r="P3" s="12"/>
       <c r="Q3" s="11"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -12067,7 +12061,7 @@
       <c r="P4" s="12"/>
       <c r="Q4" s="11"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -12082,7 +12076,7 @@
       <c r="J5" s="35"/>
       <c r="P5" s="56"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>58</v>
       </c>
@@ -12099,7 +12093,7 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="15"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="24"/>
       <c r="C8" s="66"/>
@@ -12121,7 +12115,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28"/>
       <c r="B9" s="29"/>
       <c r="C9" s="28"/>
@@ -12151,7 +12145,7 @@
       <c r="P9" s="11"/>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" spans="1:19" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="71" t="s">
         <v>10</v>
       </c>
@@ -12191,14 +12185,14 @@
       <c r="O10" s="12"/>
       <c r="P10" s="17"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="235" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="247" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="236"/>
-      <c r="C11" s="236"/>
-      <c r="D11" s="236"/>
-      <c r="E11" s="236"/>
+      <c r="B11" s="248"/>
+      <c r="C11" s="248"/>
+      <c r="D11" s="248"/>
+      <c r="E11" s="248"/>
       <c r="F11" s="108"/>
       <c r="G11" s="34"/>
       <c r="H11" s="44"/>
@@ -12211,7 +12205,7 @@
       <c r="Q11" s="51"/>
       <c r="R11" s="51"/>
     </row>
-    <row r="12" spans="1:19" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="78">
         <v>1</v>
       </c>
@@ -12249,14 +12243,14 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="8"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="237" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="249" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="238"/>
-      <c r="C13" s="238"/>
-      <c r="D13" s="238"/>
-      <c r="E13" s="238"/>
+      <c r="B13" s="250"/>
+      <c r="C13" s="250"/>
+      <c r="D13" s="250"/>
+      <c r="E13" s="250"/>
       <c r="F13" s="115"/>
       <c r="H13" s="44"/>
       <c r="I13" s="41"/>
@@ -12264,7 +12258,7 @@
       <c r="K13" s="55"/>
       <c r="L13" s="42"/>
     </row>
-    <row r="14" spans="1:19" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="81">
         <v>2</v>
       </c>
@@ -12297,7 +12291,7 @@
       <c r="K14" s="55"/>
       <c r="L14" s="42"/>
     </row>
-    <row r="15" spans="1:19" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="81">
         <v>3</v>
       </c>
@@ -12330,7 +12324,7 @@
       <c r="K15" s="55"/>
       <c r="L15" s="42"/>
     </row>
-    <row r="16" spans="1:19" ht="99.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="81">
         <v>4</v>
       </c>
@@ -12363,11 +12357,11 @@
       <c r="K16" s="55"/>
       <c r="L16" s="42"/>
     </row>
-    <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="81">
         <v>5</v>
       </c>
-      <c r="B17" s="239"/>
+      <c r="B17" s="251"/>
       <c r="C17" s="111" t="s">
         <v>49</v>
       </c>
@@ -12396,11 +12390,11 @@
       <c r="K17" s="55"/>
       <c r="L17" s="42"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="81">
         <v>6</v>
       </c>
-      <c r="B18" s="240"/>
+      <c r="B18" s="252"/>
       <c r="C18" s="112" t="s">
         <v>50</v>
       </c>
@@ -12429,11 +12423,11 @@
       <c r="K18" s="55"/>
       <c r="L18" s="42"/>
     </row>
-    <row r="19" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="81">
         <v>7</v>
       </c>
-      <c r="B19" s="241"/>
+      <c r="B19" s="253"/>
       <c r="C19" s="113" t="s">
         <v>51</v>
       </c>
@@ -12462,14 +12456,14 @@
       <c r="K19" s="55"/>
       <c r="L19" s="42"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="237" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="249" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="238"/>
-      <c r="C20" s="238"/>
-      <c r="D20" s="238"/>
-      <c r="E20" s="238"/>
+      <c r="B20" s="250"/>
+      <c r="C20" s="250"/>
+      <c r="D20" s="250"/>
+      <c r="E20" s="250"/>
       <c r="F20" s="115"/>
       <c r="H20" s="44"/>
       <c r="I20" s="41"/>
@@ -12477,7 +12471,7 @@
       <c r="K20" s="55"/>
       <c r="L20" s="42"/>
     </row>
-    <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="86">
         <v>8</v>
       </c>
@@ -12510,7 +12504,7 @@
       <c r="K21" s="55"/>
       <c r="L21" s="42"/>
     </row>
-    <row r="22" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="78">
         <v>9</v>
       </c>
@@ -12543,7 +12537,7 @@
       <c r="K22" s="55"/>
       <c r="L22" s="42"/>
     </row>
-    <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="78">
         <v>10</v>
       </c>
@@ -12576,7 +12570,7 @@
       <c r="K23" s="55"/>
       <c r="L23" s="42"/>
     </row>
-    <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="78">
         <v>11</v>
       </c>
@@ -12609,7 +12603,7 @@
       <c r="K24" s="55"/>
       <c r="L24" s="42"/>
     </row>
-    <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="78">
         <v>12</v>
       </c>
@@ -12642,7 +12636,7 @@
       <c r="K25" s="55"/>
       <c r="L25" s="42"/>
     </row>
-    <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="78">
         <v>13</v>
       </c>
@@ -12675,14 +12669,14 @@
       <c r="K26" s="55"/>
       <c r="L26" s="42"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="237" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="249" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="238"/>
-      <c r="C27" s="238"/>
-      <c r="D27" s="238"/>
-      <c r="E27" s="238"/>
+      <c r="B27" s="250"/>
+      <c r="C27" s="250"/>
+      <c r="D27" s="250"/>
+      <c r="E27" s="250"/>
       <c r="F27" s="115"/>
       <c r="H27" s="44"/>
       <c r="I27" s="41"/>
@@ -12690,11 +12684,11 @@
       <c r="K27" s="55"/>
       <c r="L27" s="42"/>
     </row>
-    <row r="28" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="78">
         <v>14</v>
       </c>
-      <c r="B28" s="242"/>
+      <c r="B28" s="254"/>
       <c r="C28" s="111" t="s">
         <v>38</v>
       </c>
@@ -12723,11 +12717,11 @@
       <c r="K28" s="55"/>
       <c r="L28" s="42"/>
     </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="78">
         <v>15</v>
       </c>
-      <c r="B29" s="244"/>
+      <c r="B29" s="256"/>
       <c r="C29" s="113" t="s">
         <v>39</v>
       </c>
@@ -12756,11 +12750,11 @@
       <c r="K29" s="55"/>
       <c r="L29" s="42"/>
     </row>
-    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="78">
         <v>16</v>
       </c>
-      <c r="B30" s="242"/>
+      <c r="B30" s="254"/>
       <c r="C30" s="111" t="s">
         <v>40</v>
       </c>
@@ -12789,11 +12783,11 @@
       <c r="K30" s="55"/>
       <c r="L30" s="42"/>
     </row>
-    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="78">
         <v>17</v>
       </c>
-      <c r="B31" s="244"/>
+      <c r="B31" s="256"/>
       <c r="C31" s="113" t="s">
         <v>41</v>
       </c>
@@ -12822,11 +12816,11 @@
       <c r="K31" s="55"/>
       <c r="L31" s="42"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="78">
         <v>18</v>
       </c>
-      <c r="B32" s="242"/>
+      <c r="B32" s="254"/>
       <c r="C32" s="83" t="s">
         <v>42</v>
       </c>
@@ -12855,11 +12849,11 @@
       <c r="K32" s="55"/>
       <c r="L32" s="42"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="78">
         <v>19</v>
       </c>
-      <c r="B33" s="243"/>
+      <c r="B33" s="255"/>
       <c r="C33" s="84" t="s">
         <v>43</v>
       </c>
@@ -12888,11 +12882,11 @@
       <c r="K33" s="55"/>
       <c r="L33" s="42"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="78">
         <v>20</v>
       </c>
-      <c r="B34" s="243"/>
+      <c r="B34" s="255"/>
       <c r="C34" s="84" t="s">
         <v>44</v>
       </c>
@@ -12921,11 +12915,11 @@
       <c r="K34" s="55"/>
       <c r="L34" s="42"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="78">
         <v>21</v>
       </c>
-      <c r="B35" s="243"/>
+      <c r="B35" s="255"/>
       <c r="C35" s="84" t="s">
         <v>45</v>
       </c>
@@ -12954,11 +12948,11 @@
       <c r="K35" s="55"/>
       <c r="L35" s="42"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="78">
         <v>22</v>
       </c>
-      <c r="B36" s="243"/>
+      <c r="B36" s="255"/>
       <c r="C36" s="84" t="s">
         <v>46</v>
       </c>
@@ -12987,11 +12981,11 @@
       <c r="K36" s="55"/>
       <c r="L36" s="42"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="78">
         <v>23</v>
       </c>
-      <c r="B37" s="243"/>
+      <c r="B37" s="255"/>
       <c r="C37" s="84" t="s">
         <v>47</v>
       </c>
@@ -13020,11 +13014,11 @@
       <c r="K37" s="55"/>
       <c r="L37" s="42"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="78">
         <v>24</v>
       </c>
-      <c r="B38" s="244"/>
+      <c r="B38" s="256"/>
       <c r="C38" s="85" t="s">
         <v>48</v>
       </c>
@@ -13053,14 +13047,14 @@
       <c r="K38" s="55"/>
       <c r="L38" s="42"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="237" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="249" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="238"/>
-      <c r="C39" s="238"/>
-      <c r="D39" s="238"/>
-      <c r="E39" s="238"/>
+      <c r="B39" s="250"/>
+      <c r="C39" s="250"/>
+      <c r="D39" s="250"/>
+      <c r="E39" s="250"/>
       <c r="F39" s="115"/>
       <c r="H39" s="44"/>
       <c r="I39" s="41"/>
@@ -13068,7 +13062,7 @@
       <c r="K39" s="55"/>
       <c r="L39" s="42"/>
     </row>
-    <row r="40" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="81">
         <v>25</v>
       </c>
@@ -13101,7 +13095,7 @@
       <c r="K40" s="55"/>
       <c r="L40" s="42"/>
     </row>
-    <row r="41" spans="1:12" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="81">
         <v>26</v>
       </c>
@@ -13134,7 +13128,7 @@
       <c r="K41" s="55"/>
       <c r="L41" s="42"/>
     </row>
-    <row r="42" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="67"/>
       <c r="H42" s="68" t="e">
         <f>SUM(H11:H41)</f>
@@ -13149,32 +13143,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" s="70"/>
       <c r="F54" s="31"/>
       <c r="G54" s="43"/>
     </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55" s="70"/>
       <c r="F55" s="31"/>
       <c r="G55" s="43"/>
     </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E56" s="70"/>
       <c r="F56" s="31"/>
       <c r="G56" s="43"/>
     </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E57" s="70"/>
       <c r="F57" s="31"/>
       <c r="G57" s="43"/>
     </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E58" s="70"/>
       <c r="F58" s="31"/>
       <c r="G58" s="43"/>
     </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E59" s="70"/>
       <c r="F59" s="31"/>
       <c r="G59" s="43"/>

</xml_diff>